<commit_message>
- Merge axes and SAM inputs/outputs
</commit_message>
<xml_diff>
--- a/branches/multirun/example/Vegetative_stages/inputs/Generate_inputs.xlsx
+++ b/branches/multirun/example/Vegetative_stages/inputs/Generate_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="INPUTS" sheetId="15" r:id="rId1"/>
@@ -760,15 +760,9 @@
     <t>U (kg N/ha)</t>
   </si>
   <si>
-    <t>g.m-2</t>
-  </si>
-  <si>
     <t>Apport 01/04</t>
   </si>
   <si>
-    <t>nitrates (µmon N.m-2)</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -830,6 +824,12 @@
   </si>
   <si>
     <t>mean_conc_sucrose</t>
+  </si>
+  <si>
+    <t>nitrates (µmol N.m-3)</t>
+  </si>
+  <si>
+    <t>g.m-3</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1251,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1361,7 +1361,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1728,11 +1727,11 @@
       <c r="E1" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="W1" s="93" t="s">
-        <v>172</v>
-      </c>
-      <c r="X1" s="94" t="s">
-        <v>173</v>
+      <c r="W1" s="92" t="s">
+        <v>170</v>
+      </c>
+      <c r="X1" s="93" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:55" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1747,15 +1746,15 @@
         <f xml:space="preserve"> 76.1/12*24*3600</f>
         <v>547920</v>
       </c>
-      <c r="W2" s="95">
+      <c r="W2" s="94">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="X2" s="95">
+      <c r="X2" s="94">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="4" spans="1:55" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="98" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1822,7 +1821,7 @@
         <v>13</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="X4" s="5" t="s">
         <v>14</v>
@@ -1875,8 +1874,8 @@
       <c r="AN4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AO4" s="97" t="s">
-        <v>179</v>
+      <c r="AO4" s="96" t="s">
+        <v>177</v>
       </c>
       <c r="AP4" s="12" t="s">
         <v>77</v>
@@ -1894,10 +1893,10 @@
         <v>24</v>
       </c>
       <c r="AU4" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="AV4" s="86" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="AV4" s="85" t="s">
+        <v>160</v>
       </c>
       <c r="AW4" s="6" t="s">
         <v>63</v>
@@ -1920,7 +1919,7 @@
       </c>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A5" s="99"/>
+      <c r="A5" s="98"/>
       <c r="B5">
         <v>1</v>
       </c>
@@ -2014,19 +2013,19 @@
         <v>33</v>
       </c>
       <c r="AE5" s="1">
-        <f>AK5*$AQ$15</f>
+        <f t="shared" ref="AE5:AE12" si="0">AK5*$AQ$15</f>
         <v>8.9088436646547198</v>
       </c>
       <c r="AF5" s="1">
-        <f>AK5*$AS5</f>
+        <f t="shared" ref="AF5:AF12" si="1">AK5*$AS5</f>
         <v>0.99652622317307915</v>
       </c>
       <c r="AG5" s="24">
-        <f>AK5*$AV5</f>
+        <f t="shared" ref="AG5:AG12" si="2">AK5*$AV5</f>
         <v>8.9088436646547198</v>
       </c>
       <c r="AH5" s="28">
-        <f>AK5*$AT5</f>
+        <f t="shared" ref="AH5:AH12" si="3">AK5*$AT5</f>
         <v>9.9652622317307902</v>
       </c>
       <c r="AI5" s="1">
@@ -2057,29 +2056,29 @@
         <v>1800</v>
       </c>
       <c r="AP5" s="58">
-        <f>AK5+AE5*$E$31+AF5*$F$31+AH5*$J$31</f>
+        <f t="shared" ref="AP5:AP12" si="4">AK5+AE5*$E$31+AF5*$F$31+AH5*$J$31</f>
         <v>3.3011513455652687E-3</v>
       </c>
       <c r="AQ5" s="59">
-        <f>(1-AK5/AP5)*100</f>
+        <f t="shared" ref="AQ5:AQ12" si="5">(1-AK5/AP5)*100</f>
         <v>38.829284515098252</v>
       </c>
       <c r="AR5" s="13">
         <v>4.5999999999999996</v>
       </c>
       <c r="AS5" s="13">
-        <f>(($AR5/100)*(1+($AQ$15+$AV5)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR5/100))</f>
+        <f t="shared" ref="AS5:AS12" si="6">(($AR5/100)*(1+($AQ$15+$AV5)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR5/100))</f>
         <v>493.49156696102204</v>
       </c>
       <c r="AT5" s="13">
-        <f>$AS5/$X$23</f>
+        <f t="shared" ref="AT5:AT12" si="7">$AS5/$X$23</f>
         <v>4934.91566961022</v>
       </c>
       <c r="AU5" s="13">
         <v>10</v>
       </c>
       <c r="AV5" s="71">
-        <f>$AU5/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" ref="AV5:AV12" si="8">$AU5/100/(1-$X$33)*$X$32*10^6/$X$30</f>
         <v>4411.7647058823532</v>
       </c>
       <c r="AW5" s="7">
@@ -2090,7 +2089,7 @@
         <v>9.1058115591388438E-4</v>
       </c>
       <c r="AY5" s="7">
-        <f>J5*Z5</f>
+        <f t="shared" ref="AY5:AY12" si="9">J5*Z5</f>
         <v>2.6054999999999997E-3</v>
       </c>
       <c r="AZ5" s="8">
@@ -2098,17 +2097,17 @@
         <v>2.0180134110471437E-3</v>
       </c>
       <c r="BA5" s="8">
-        <f>$T$27+$T$28*$T$30*(L5)^$T$29</f>
+        <f t="shared" ref="BA5:BA12" si="10">$T$27+$T$28*$T$30*(L5)^$T$29</f>
         <v>4.0277279389003447E-3</v>
       </c>
       <c r="BB5" s="7"/>
       <c r="BC5" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M5)^$AW$21</f>
+        <f t="shared" ref="BC5:BC12" si="11">$AX$20*$AW$22*$AW$24*(M5)^$AW$21</f>
         <v>1.3244862745926676E-6</v>
       </c>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A6" s="99"/>
+      <c r="A6" s="98"/>
       <c r="B6">
         <v>1</v>
       </c>
@@ -2119,7 +2118,7 @@
         <v>4</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E11" si="0">(10-D6)*$E$2</f>
+        <f t="shared" ref="E6:E11" si="12">(10-D6)*$E$2</f>
         <v>3287520</v>
       </c>
       <c r="F6">
@@ -2139,7 +2138,7 @@
         <v>2.894E-2</v>
       </c>
       <c r="K6" s="38">
-        <f t="shared" ref="K6:K12" si="1">J6-M6</f>
+        <f t="shared" ref="K6:K12" si="13">J6-M6</f>
         <v>2.8930000000000001E-2</v>
       </c>
       <c r="L6" s="38">
@@ -2176,7 +2175,7 @@
         <v>3.3993521965748258E-2</v>
       </c>
       <c r="W6" s="1">
-        <f t="shared" ref="W6:W12" si="2">$W$2*EXP($X$2*E6)</f>
+        <f t="shared" ref="W6:W12" si="14">$W$2*EXP($X$2*E6)</f>
         <v>2.6776375833009532E-5</v>
       </c>
       <c r="X6" t="s">
@@ -2201,19 +2200,19 @@
         <v>33</v>
       </c>
       <c r="AE6" s="1">
-        <f>AK6*$AQ$15</f>
+        <f t="shared" si="0"/>
         <v>3.5881220853167113</v>
       </c>
       <c r="AF6" s="1">
-        <f>AK6*$AS6</f>
+        <f t="shared" si="1"/>
         <v>0.67583627559825854</v>
       </c>
       <c r="AG6" s="24">
-        <f>AK6*$AV6</f>
+        <f t="shared" si="2"/>
         <v>1.7940610426583556</v>
       </c>
       <c r="AH6" s="28">
-        <f>AK6*$AT6</f>
+        <f t="shared" si="3"/>
         <v>6.7583627559825858</v>
       </c>
       <c r="AI6" s="1">
@@ -2225,48 +2224,48 @@
         <v>1.6879744031468265E-7</v>
       </c>
       <c r="AK6">
-        <f t="shared" ref="AK6:AK12" si="3">AI6+AJ6</f>
+        <f t="shared" ref="AK6:AK12" si="15">AI6+AJ6</f>
         <v>8.1330767267178783E-4</v>
       </c>
       <c r="AL6">
-        <f t="shared" ref="AL6:AM12" si="4">AI6*0.005</f>
+        <f t="shared" ref="AL6:AM12" si="16">AI6*0.005</f>
         <v>4.0656943761573658E-6</v>
       </c>
       <c r="AM6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>8.4398720157341326E-10</v>
       </c>
       <c r="AN6">
-        <f t="shared" ref="AN6:AN12" si="5">AL6+AM6</f>
+        <f t="shared" ref="AN6:AN12" si="17">AL6+AM6</f>
         <v>4.066538363358939E-6</v>
       </c>
       <c r="AO6" s="1">
         <v>1800</v>
       </c>
       <c r="AP6" s="58">
-        <f>AK6+AE6*$E$31+AF6*$F$31+AH6*$J$31</f>
+        <f t="shared" si="4"/>
         <v>1.612515340843685E-3</v>
       </c>
       <c r="AQ6" s="59">
-        <f>(1-AK6/AP6)*100</f>
+        <f t="shared" si="5"/>
         <v>49.562794717583479</v>
       </c>
       <c r="AR6" s="13">
         <v>6.5</v>
       </c>
       <c r="AS6" s="13">
-        <f>(($AR6/100)*(1+($AQ$15+$AV6)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR6/100))</f>
+        <f t="shared" si="6"/>
         <v>830.97245766546928</v>
       </c>
       <c r="AT6" s="13">
-        <f>$AS6/$X$23</f>
+        <f t="shared" si="7"/>
         <v>8309.724576654693</v>
       </c>
       <c r="AU6" s="13">
         <v>5</v>
       </c>
       <c r="AV6" s="71">
-        <f>$AU6/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>2205.8823529411766</v>
       </c>
       <c r="AW6" s="7">
@@ -2277,7 +2276,7 @@
         <v>9.1017858127080242E-4</v>
       </c>
       <c r="AY6" s="7" t="e">
-        <f>J6*Z6</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ6" s="8" t="e">
@@ -2285,17 +2284,17 @@
         <v>#VALUE!</v>
       </c>
       <c r="BA6" s="8">
-        <f>$T$27+$T$28*$T$30*(L6)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>8.1313887523147316E-4</v>
       </c>
       <c r="BB6" s="7"/>
       <c r="BC6" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M6)^$AW$21</f>
+        <f t="shared" si="11"/>
         <v>1.6879744031468265E-7</v>
       </c>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A7" s="99"/>
+      <c r="A7" s="98"/>
       <c r="B7">
         <v>1</v>
       </c>
@@ -2306,7 +2305,7 @@
         <v>5</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>2739600</v>
       </c>
       <c r="F7">
@@ -2326,7 +2325,7 @@
         <v>2.894E-2</v>
       </c>
       <c r="K7" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
       <c r="L7" s="38">
@@ -2363,7 +2362,7 @@
         <v>32</v>
       </c>
       <c r="W7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1.5480791541095022E-5</v>
       </c>
       <c r="X7" t="s">
@@ -2388,19 +2387,19 @@
         <v>33</v>
       </c>
       <c r="AE7" s="1">
-        <f>AK7*$AQ$15</f>
+        <f t="shared" si="0"/>
         <v>0.13143561599020981</v>
       </c>
       <c r="AF7" s="1">
-        <f>AK7*$AS7</f>
+        <f t="shared" si="1"/>
         <v>5.4184269937105296E-2</v>
       </c>
       <c r="AG7" s="24">
-        <f>AK7*$AV7</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH7" s="28">
-        <f>AK7*$AT7</f>
+        <f t="shared" si="3"/>
         <v>0.54184269937105289</v>
       </c>
       <c r="AI7" s="1">
@@ -2411,75 +2410,75 @@
         <v>0</v>
       </c>
       <c r="AK7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>2.9792072957780891E-5</v>
       </c>
       <c r="AL7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>1.4896036478890447E-7</v>
       </c>
       <c r="AM7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AN7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="17"/>
         <v>1.4896036478890447E-7</v>
       </c>
       <c r="AO7" s="1">
         <v>1800</v>
       </c>
       <c r="AP7" s="58">
-        <f>AK7+AE7*$E$31+AF7*$F$31+AH7*$J$31</f>
+        <f t="shared" si="4"/>
         <v>8.9403557211611783E-5</v>
       </c>
       <c r="AQ7" s="59">
-        <f>(1-AK7/AP7)*100</f>
+        <f t="shared" si="5"/>
         <v>66.676859526668281</v>
       </c>
       <c r="AR7" s="13">
         <v>9.5</v>
       </c>
       <c r="AS7" s="13">
-        <f>(($AR7/100)*(1+($AQ$15+$AV7)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR7/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AT7" s="13">
-        <f>$AS7/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AU7" s="13">
         <v>0</v>
       </c>
       <c r="AV7" s="71">
-        <f>$AU7/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW7" s="7"/>
       <c r="AX7" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T7*$T$32)^$T$29</f>
+        <f t="shared" ref="AX7:AX12" si="18">$T$27+$T$28*$T$30*(T7*$T$32)^$T$29</f>
         <v>#VALUE!</v>
       </c>
       <c r="AY7" s="7" t="e">
-        <f>J7*Z7</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ7" s="8" t="e">
-        <f>AX7+((AY7-AX7)/$T$31)*F7</f>
+        <f t="shared" ref="AZ7:AZ12" si="19">AX7+((AY7-AX7)/$T$31)*F7</f>
         <v>#VALUE!</v>
       </c>
       <c r="BA7" s="8">
-        <f>$T$27+$T$28*$T$30*(L7)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>2.9792072957780891E-5</v>
       </c>
       <c r="BB7" s="7"/>
       <c r="BC7" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M7)^$AW$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A8" s="99"/>
+      <c r="A8" s="98"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -2490,7 +2489,7 @@
         <v>6</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>2191680</v>
       </c>
       <c r="F8">
@@ -2506,11 +2505,11 @@
         <v>33</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:J12" si="6">J7-M8</f>
+        <f t="shared" ref="J8:J12" si="20">J7-M8</f>
         <v>2.894E-2</v>
       </c>
       <c r="K8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
       <c r="L8" s="38">
@@ -2547,7 +2546,7 @@
         <v>32</v>
       </c>
       <c r="W8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>8.9502368891684043E-6</v>
       </c>
       <c r="X8" t="s">
@@ -2572,98 +2571,98 @@
         <v>33</v>
       </c>
       <c r="AE8" s="1">
-        <f>AK8*$AQ$15</f>
+        <f t="shared" si="0"/>
         <v>3.5630437425207336E-2</v>
       </c>
       <c r="AF8" s="1">
-        <f>AK8*$AS8</f>
+        <f t="shared" si="1"/>
         <v>1.4688630816538933E-2</v>
       </c>
       <c r="AG8" s="24">
-        <f>AK8*$AV8</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH8" s="28">
-        <f>AK8*$AT8</f>
+        <f t="shared" si="3"/>
         <v>0.14688630816538931</v>
       </c>
       <c r="AI8" s="1">
-        <f t="shared" ref="AI8:AI12" si="7">BA8</f>
+        <f t="shared" ref="AI8:AI12" si="21">BA8</f>
         <v>8.076232483046996E-6</v>
       </c>
       <c r="AJ8" s="1">
         <v>0</v>
       </c>
       <c r="AK8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>8.076232483046996E-6</v>
       </c>
       <c r="AL8">
+        <f t="shared" si="16"/>
+        <v>4.0381162415234981E-8</v>
+      </c>
+      <c r="AM8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <f t="shared" si="17"/>
+        <v>4.0381162415234981E-8</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP8" s="58">
         <f t="shared" si="4"/>
-        <v>4.0381162415234981E-8</v>
-      </c>
-      <c r="AM8">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AN8">
+        <v>2.4236108506970847E-5</v>
+      </c>
+      <c r="AQ8" s="59">
         <f t="shared" si="5"/>
-        <v>4.0381162415234981E-8</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP8" s="58">
-        <f>AK8+AE8*$E$31+AF8*$F$31+AH8*$J$31</f>
-        <v>2.4236108506970847E-5</v>
-      </c>
-      <c r="AQ8" s="59">
-        <f>(1-AK8/AP8)*100</f>
         <v>66.676859526668281</v>
       </c>
       <c r="AR8" s="13">
         <v>9.5</v>
       </c>
       <c r="AS8" s="13">
-        <f>(($AR8/100)*(1+($AQ$15+$AV8)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR8/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AT8" s="13">
-        <f>$AS8/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AU8" s="13">
         <v>0</v>
       </c>
       <c r="AV8" s="71">
-        <f>$AU8/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW8" s="7"/>
       <c r="AX8" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T8*$T$32)^$T$29</f>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="AY8" s="7" t="e">
-        <f>J8*Z8</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ8" s="8" t="e">
-        <f>AX8+((AY8-AX8)/$T$31)*F8</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BA8" s="8">
-        <f>$T$27+$T$28*$T$30*(L8)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>8.076232483046996E-6</v>
       </c>
       <c r="BB8" s="7"/>
       <c r="BC8" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M8)^$AW$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A9" s="99"/>
+      <c r="A9" s="98"/>
       <c r="B9">
         <v>1</v>
       </c>
@@ -2674,7 +2673,7 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>1643760</v>
       </c>
       <c r="F9">
@@ -2690,11 +2689,11 @@
         <v>33</v>
       </c>
       <c r="J9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="20"/>
         <v>2.894E-2</v>
       </c>
       <c r="K9" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
       <c r="L9" s="38">
@@ -2731,7 +2730,7 @@
         <v>32</v>
       </c>
       <c r="W9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>5.1745894361784425E-6</v>
       </c>
       <c r="X9" t="s">
@@ -2756,98 +2755,98 @@
         <v>33</v>
       </c>
       <c r="AE9" s="1">
-        <f>AK9*$AQ$15</f>
+        <f t="shared" si="0"/>
         <v>1.2193691971899337E-2</v>
       </c>
       <c r="AF9" s="1">
-        <f>AK9*$AS9</f>
+        <f t="shared" si="1"/>
         <v>5.0268436934515614E-3</v>
       </c>
       <c r="AG9" s="24">
-        <f>AK9*$AV9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH9" s="28">
-        <f>AK9*$AT9</f>
+        <f t="shared" si="3"/>
         <v>5.026843693451561E-2</v>
       </c>
       <c r="AI9" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>2.7639035136305163E-6</v>
       </c>
       <c r="AJ9" s="1">
         <v>0</v>
       </c>
       <c r="AK9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>2.7639035136305163E-6</v>
       </c>
       <c r="AL9">
+        <f t="shared" si="16"/>
+        <v>1.3819517568152583E-8</v>
+      </c>
+      <c r="AM9">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <f t="shared" si="17"/>
+        <v>1.3819517568152583E-8</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP9" s="58">
         <f t="shared" si="4"/>
-        <v>1.3819517568152583E-8</v>
-      </c>
-      <c r="AM9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AN9">
+        <v>8.294246803786242E-6</v>
+      </c>
+      <c r="AQ9" s="59">
         <f t="shared" si="5"/>
-        <v>1.3819517568152583E-8</v>
-      </c>
-      <c r="AO9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP9" s="58">
-        <f>AK9+AE9*$E$31+AF9*$F$31+AH9*$J$31</f>
-        <v>8.294246803786242E-6</v>
-      </c>
-      <c r="AQ9" s="59">
-        <f>(1-AK9/AP9)*100</f>
         <v>66.676859526668281</v>
       </c>
       <c r="AR9" s="13">
         <v>9.5</v>
       </c>
       <c r="AS9" s="13">
-        <f>(($AR9/100)*(1+($AQ$15+$AV9)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR9/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AT9" s="13">
-        <f>$AS9/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AU9" s="13">
         <v>0</v>
       </c>
       <c r="AV9" s="71">
-        <f>$AU9/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW9" s="7"/>
       <c r="AX9" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T9*$T$32)^$T$29</f>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="AY9" s="7" t="e">
-        <f>J9*Z9</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ9" s="8" t="e">
-        <f>AX9+((AY9-AX9)/$T$31)*F9</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BA9" s="8">
-        <f>$T$27+$T$28*$T$30*(L9)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>2.7639035136305163E-6</v>
       </c>
       <c r="BB9" s="7"/>
       <c r="BC9" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M9)^$AW$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A10" s="99"/>
+      <c r="A10" s="98"/>
       <c r="B10">
         <v>1</v>
       </c>
@@ -2858,7 +2857,7 @@
         <v>8</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>1095840</v>
       </c>
       <c r="F10">
@@ -2874,11 +2873,11 @@
         <v>33</v>
       </c>
       <c r="J10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="20"/>
         <v>2.894E-2</v>
       </c>
       <c r="K10" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
       <c r="L10" s="38">
@@ -2915,7 +2914,7 @@
         <v>32</v>
       </c>
       <c r="W10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>2.9916946517264094E-6</v>
       </c>
       <c r="X10" t="s">
@@ -2940,98 +2939,98 @@
         <v>33</v>
       </c>
       <c r="AE10" s="1">
-        <f>AK10*$AQ$15</f>
+        <f t="shared" si="0"/>
         <v>5.2963394285683064E-3</v>
       </c>
       <c r="AF10" s="1">
-        <f>AK10*$AS10</f>
+        <f t="shared" si="1"/>
         <v>2.1834134006527969E-3</v>
       </c>
       <c r="AG10" s="24">
-        <f>AK10*$AV10</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH10" s="28">
-        <f>AK10*$AT10</f>
+        <f t="shared" si="3"/>
         <v>2.1834134006527964E-2</v>
       </c>
       <c r="AI10" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>1.2005036038088161E-6</v>
       </c>
       <c r="AJ10" s="1">
         <v>0</v>
       </c>
       <c r="AK10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>1.2005036038088161E-6</v>
       </c>
       <c r="AL10">
+        <f t="shared" si="16"/>
+        <v>6.0025180190440811E-9</v>
+      </c>
+      <c r="AM10">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <f t="shared" si="17"/>
+        <v>6.0025180190440811E-9</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP10" s="58">
         <f t="shared" si="4"/>
-        <v>6.0025180190440811E-9</v>
-      </c>
-      <c r="AM10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AN10">
+        <v>3.6026124391534188E-6</v>
+      </c>
+      <c r="AQ10" s="59">
         <f t="shared" si="5"/>
-        <v>6.0025180190440811E-9</v>
-      </c>
-      <c r="AO10" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP10" s="58">
-        <f>AK10+AE10*$E$31+AF10*$F$31+AH10*$J$31</f>
-        <v>3.6026124391534188E-6</v>
-      </c>
-      <c r="AQ10" s="59">
-        <f>(1-AK10/AP10)*100</f>
         <v>66.676859526668281</v>
       </c>
       <c r="AR10" s="13">
         <v>9.5</v>
       </c>
       <c r="AS10" s="13">
-        <f>(($AR10/100)*(1+($AQ$15+$AV10)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR10/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AT10" s="13">
-        <f>$AS10/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AU10" s="13">
         <v>0</v>
       </c>
       <c r="AV10" s="71">
-        <f>$AU10/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW10" s="7"/>
       <c r="AX10" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T10*$T$32)^$T$29</f>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="AY10" s="7" t="e">
-        <f>J10*Z10</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ10" s="8" t="e">
-        <f>AX10+((AY10-AX10)/$T$31)*F10</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BA10" s="8">
-        <f>$T$27+$T$28*$T$30*(L10)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>1.2005036038088161E-6</v>
       </c>
       <c r="BB10" s="7"/>
       <c r="BC10" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M10)^$AW$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A11" s="99"/>
+      <c r="A11" s="98"/>
       <c r="B11">
         <v>1</v>
       </c>
@@ -3042,7 +3041,7 @@
         <v>9</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>547920</v>
       </c>
       <c r="F11">
@@ -3058,11 +3057,11 @@
         <v>33</v>
       </c>
       <c r="J11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="20"/>
         <v>2.894E-2</v>
       </c>
       <c r="K11" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
       <c r="L11" s="39">
@@ -3099,7 +3098,7 @@
         <v>32</v>
       </c>
       <c r="W11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1.7296515983649451E-6</v>
       </c>
       <c r="X11" t="s">
@@ -3124,98 +3123,98 @@
         <v>33</v>
       </c>
       <c r="AE11" s="1">
-        <f>AK11*$AQ$15</f>
+        <f t="shared" si="0"/>
         <v>1.9146799290632522E-3</v>
       </c>
       <c r="AF11" s="1">
-        <f>AK11*$AS11</f>
+        <f t="shared" si="1"/>
         <v>7.8932588657893549E-4</v>
       </c>
       <c r="AG11" s="24">
-        <f>AK11*$AV11</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH11" s="28">
-        <f>AK11*$AT11</f>
+        <f t="shared" si="3"/>
         <v>7.8932588657893536E-3</v>
       </c>
       <c r="AI11" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>4.3399411725433714E-7</v>
       </c>
       <c r="AJ11" s="1">
         <v>0</v>
       </c>
       <c r="AK11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>4.3399411725433714E-7</v>
       </c>
       <c r="AL11">
+        <f t="shared" si="16"/>
+        <v>2.1699705862716857E-9</v>
+      </c>
+      <c r="AM11">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <f t="shared" si="17"/>
+        <v>2.1699705862716857E-9</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP11" s="58">
         <f t="shared" si="4"/>
-        <v>2.1699705862716857E-9</v>
-      </c>
-      <c r="AM11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AN11">
+        <v>1.3023806012571343E-6</v>
+      </c>
+      <c r="AQ11" s="59">
         <f t="shared" si="5"/>
-        <v>2.1699705862716857E-9</v>
-      </c>
-      <c r="AO11" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP11" s="58">
-        <f>AK11+AE11*$E$31+AF11*$F$31+AH11*$J$31</f>
-        <v>1.3023806012571343E-6</v>
-      </c>
-      <c r="AQ11" s="59">
-        <f>(1-AK11/AP11)*100</f>
         <v>66.676859526668281</v>
       </c>
       <c r="AR11" s="13">
         <v>9.5</v>
       </c>
       <c r="AS11" s="13">
-        <f>(($AR11/100)*(1+($AQ$15+$AV11)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR11/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AT11" s="13">
-        <f>$AS11/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AU11" s="13">
         <v>0</v>
       </c>
       <c r="AV11" s="71">
-        <f>$AU11/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW11" s="7"/>
       <c r="AX11" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T11*$T$32)^$T$29</f>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="AY11" s="7" t="e">
-        <f>J11*Z11</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ11" s="8" t="e">
-        <f>AX11+((AY11-AX11)/$T$31)*F11</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BA11" s="8">
-        <f>$T$27+$T$28*$T$30*(L11)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>4.3399411725433714E-7</v>
       </c>
       <c r="BB11" s="7"/>
       <c r="BC11" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M11)^$AW$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A12" s="99"/>
+      <c r="A12" s="98"/>
       <c r="B12">
         <v>1</v>
       </c>
@@ -3242,11 +3241,11 @@
         <v>33</v>
       </c>
       <c r="J12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="20"/>
         <v>2.894E-2</v>
       </c>
       <c r="K12" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
       <c r="L12" s="39">
@@ -3283,7 +3282,7 @@
         <v>32</v>
       </c>
       <c r="W12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="X12" t="s">
@@ -3308,93 +3307,93 @@
         <v>33</v>
       </c>
       <c r="AE12" s="1">
-        <f>AK12*$AQ$15</f>
+        <f t="shared" si="0"/>
         <v>1.2855761246405892E-3</v>
       </c>
       <c r="AF12" s="1">
-        <f>AK12*$AS12</f>
+        <f t="shared" si="1"/>
         <v>5.2997814357572592E-4</v>
       </c>
       <c r="AG12" s="24">
-        <f>AK12*$AV12</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH12" s="28">
-        <f>AK12*$AT12</f>
+        <f t="shared" si="3"/>
         <v>5.2997814357572583E-3</v>
       </c>
       <c r="AI12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>2.9139725491853351E-7</v>
       </c>
       <c r="AJ12" s="1">
         <v>0</v>
       </c>
       <c r="AK12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>2.9139725491853351E-7</v>
       </c>
       <c r="AL12">
+        <f t="shared" si="16"/>
+        <v>1.4569862745926675E-9</v>
+      </c>
+      <c r="AM12">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AN12">
+        <f t="shared" si="17"/>
+        <v>1.4569862745926675E-9</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP12" s="61">
         <f t="shared" si="4"/>
-        <v>1.4569862745926675E-9</v>
-      </c>
-      <c r="AM12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AN12">
+        <v>8.7445916195004701E-7</v>
+      </c>
+      <c r="AQ12" s="60">
         <f t="shared" si="5"/>
-        <v>1.4569862745926675E-9</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP12" s="61">
-        <f>AK12+AE12*$E$31+AF12*$F$31+AH12*$J$31</f>
-        <v>8.7445916195004701E-7</v>
-      </c>
-      <c r="AQ12" s="60">
-        <f>(1-AK12/AP12)*100</f>
         <v>66.676859526668281</v>
       </c>
       <c r="AR12" s="14">
         <v>9.5</v>
       </c>
       <c r="AS12" s="13">
-        <f>(($AR12/100)*(1+($AQ$15+$AV12)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR12/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AT12" s="14">
-        <f>$AS12/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AU12" s="14">
         <v>0</v>
       </c>
       <c r="AV12" s="71">
-        <f>$AU12/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW12" s="7"/>
       <c r="AX12" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T12*$T$32)^$T$29</f>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="AY12" s="7" t="e">
-        <f>J12*Z12</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ12" s="8" t="e">
-        <f>AX12+((AY12-AX12)/$T$31)*F12</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BA12" s="8">
-        <f>$T$27+$T$28*$T$30*(L12)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>2.9139725491853351E-7</v>
       </c>
       <c r="BB12" s="7"/>
       <c r="BC12" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M12)^$AW$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3411,7 +3410,7 @@
       <c r="AF13" s="1"/>
     </row>
     <row r="14" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="99" t="s">
+      <c r="A14" s="98" t="s">
         <v>71</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -3512,7 +3511,7 @@
       <c r="AU14" s="40"/>
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A15" s="99"/>
+      <c r="A15" s="98"/>
       <c r="B15">
         <v>1</v>
       </c>
@@ -3551,15 +3550,15 @@
         <v>1.6239747221660625</v>
       </c>
       <c r="M15">
-        <f t="shared" ref="M15:M20" si="8">J15*$X15</f>
+        <f t="shared" ref="M15:M20" si="22">J15*$X15</f>
         <v>16.239747221660625</v>
       </c>
       <c r="N15">
-        <f t="shared" ref="N15:N20" si="9">AA15*$J15</f>
+        <f t="shared" ref="N15:N20" si="23">AA15*$J15</f>
         <v>0</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" ref="O15:O20" si="10">J15*$AB$16</f>
+        <f t="shared" ref="O15:O20" si="24">J15*$AB$16</f>
         <v>18.09675</v>
       </c>
       <c r="P15">
@@ -3585,7 +3584,7 @@
         <v>4.3</v>
       </c>
       <c r="W15" s="13">
-        <f t="shared" ref="W15:W20" si="11">(($V15/100)*(1+$AB$16*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$V15/100))</f>
+        <f t="shared" ref="W15:W20" si="25">(($V15/100)*(1+$AB$16*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$V15/100))</f>
         <v>395.90503059926971</v>
       </c>
       <c r="X15" s="13">
@@ -3599,7 +3598,7 @@
         <v>27</v>
       </c>
       <c r="AA15" s="76">
-        <f t="shared" ref="AA15:AA20" si="12">IF(F15="HiddenElement",$AA$22/100/(1-$X$33)*$X$32*10^6/$X$30,0)</f>
+        <f t="shared" ref="AA15:AA20" si="26">IF(F15="HiddenElement",$AA$22/100/(1-$X$33)*$X$32*10^6/$X$30,0)</f>
         <v>0</v>
       </c>
       <c r="AB15" s="75" t="s">
@@ -3631,11 +3630,11 @@
         <f>AR15+AQ15</f>
         <v>8823.5294117647063</v>
       </c>
-      <c r="AT15" s="84"/>
-      <c r="AU15" s="84"/>
+      <c r="AT15" s="83"/>
+      <c r="AU15" s="83"/>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A16" s="99"/>
+      <c r="A16" s="98"/>
       <c r="B16">
         <v>1</v>
       </c>
@@ -3666,7 +3665,7 @@
         <v>1.7099999999999999E-3</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K16:K20" si="13">J16*0.005</f>
+        <f t="shared" ref="K16:K20" si="27">J16*0.005</f>
         <v>8.5499999999999995E-6</v>
       </c>
       <c r="L16">
@@ -3674,22 +3673,22 @@
         <v>0.19277131424832977</v>
       </c>
       <c r="M16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>1.9277131424832974</v>
       </c>
       <c r="N16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="O16" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>7.5441176470588234</v>
       </c>
       <c r="P16">
         <v>2.6861000000000002E-4</v>
       </c>
       <c r="Q16" s="1">
-        <f t="shared" ref="Q16:Q20" si="14">J16*$AC16</f>
+        <f t="shared" ref="Q16:Q20" si="28">J16*$AC16</f>
         <v>2.7359999999999999E-2</v>
       </c>
       <c r="R16">
@@ -3709,7 +3708,7 @@
         <v>1.8</v>
       </c>
       <c r="W16" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>112.73176271832151</v>
       </c>
       <c r="X16" s="13">
@@ -3723,7 +3722,7 @@
         <v>1</v>
       </c>
       <c r="AA16" s="76">
-        <f t="shared" si="12"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AB16" s="45">
@@ -3731,15 +3730,15 @@
         <v>4411.7647058823532</v>
       </c>
       <c r="AC16" s="13">
-        <f t="shared" ref="AC16:AC20" si="15">ROUND(X16/$AT$6*120,0)</f>
+        <f t="shared" ref="AC16:AC20" si="29">ROUND(X16/$AT$6*120,0)</f>
         <v>16</v>
       </c>
       <c r="AD16" s="13">
-        <f t="shared" ref="AD16:AD20" si="16">J16+L16*$F$31+M16*$J$31+O16*$E$31</f>
+        <f t="shared" ref="AD16:AD20" si="30">J16+L16*$F$31+M16*$J$31+O16*$E$31</f>
         <v>2.1242656885690431E-3</v>
       </c>
       <c r="AE16" s="59">
-        <f t="shared" ref="AE16:AE20" si="17">(1-J16/AD16)*100</f>
+        <f t="shared" ref="AE16:AE20" si="31">(1-J16/AD16)*100</f>
         <v>19.501594871030591</v>
       </c>
       <c r="AF16" s="1"/>
@@ -3756,11 +3755,11 @@
         <f>AR16+AQ16</f>
         <v>20</v>
       </c>
-      <c r="AT16" s="85"/>
-      <c r="AU16" s="85"/>
+      <c r="AT16" s="84"/>
+      <c r="AU16" s="84"/>
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A17" s="99"/>
+      <c r="A17" s="98"/>
       <c r="B17">
         <v>1</v>
       </c>
@@ -3791,23 +3790,23 @@
         <v>5.0624699999999995E-3</v>
       </c>
       <c r="K17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="27"/>
         <v>2.5312349999999998E-5</v>
       </c>
       <c r="L17">
-        <f t="shared" ref="L17:L20" si="18">J17*$W17</f>
+        <f t="shared" ref="L17:L20" si="32">J17*$W17</f>
         <v>2.3758024102824513</v>
       </c>
       <c r="M17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>23.758024102824514</v>
       </c>
       <c r="N17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>22.334426470588234</v>
       </c>
       <c r="P17">
@@ -3833,38 +3832,38 @@
         <v>4.8</v>
       </c>
       <c r="W17" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>469.29708428542818</v>
       </c>
       <c r="X17" s="13">
-        <f t="shared" ref="X17:X20" si="19">$W17/$X$23</f>
+        <f t="shared" ref="X17:X20" si="33">$W17/$X$23</f>
         <v>4692.9708428542817</v>
       </c>
       <c r="Z17" s="24"/>
       <c r="AA17" s="76">
-        <f t="shared" si="12"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AB17" s="42">
         <v>10</v>
       </c>
       <c r="AC17" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>68</v>
       </c>
       <c r="AD17" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="30"/>
         <v>8.1497066913228666E-3</v>
       </c>
       <c r="AE17" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>37.88156811348685</v>
       </c>
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A18" s="99"/>
+      <c r="A18" s="98"/>
       <c r="B18">
         <v>1</v>
       </c>
@@ -3895,30 +3894,30 @@
         <v>2.2800000000000003E-3</v>
       </c>
       <c r="K18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="27"/>
         <v>1.1400000000000003E-5</v>
       </c>
       <c r="L18">
-        <f t="shared" si="18"/>
+        <f t="shared" si="32"/>
         <v>0.36572238936056839</v>
       </c>
       <c r="M18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>3.6572238936056838</v>
       </c>
       <c r="N18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>3.0176470588235293</v>
       </c>
       <c r="O18" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>10.058823529411766</v>
       </c>
       <c r="P18">
         <v>2.4800000000000001E-4</v>
       </c>
       <c r="Q18" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>5.2440000000000007E-2</v>
       </c>
       <c r="R18">
@@ -3938,11 +3937,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="W18" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>160.40455673709138</v>
       </c>
       <c r="X18" s="13">
-        <f t="shared" si="19"/>
+        <f t="shared" si="33"/>
         <v>1604.0455673709137</v>
       </c>
       <c r="AA18" s="76">
@@ -3953,22 +3952,22 @@
         <v>120</v>
       </c>
       <c r="AC18" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>23</v>
       </c>
       <c r="AD18" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="30"/>
         <v>2.9444020852838065E-3</v>
       </c>
       <c r="AE18" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>22.564923744773314</v>
       </c>
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A19" s="99"/>
+      <c r="A19" s="98"/>
       <c r="B19">
         <v>1</v>
       </c>
@@ -3999,30 +3998,30 @@
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="K19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="27"/>
         <v>2.0000000000000002E-7</v>
       </c>
       <c r="L19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="32"/>
         <v>6.4161822694836562E-3</v>
       </c>
       <c r="M19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>6.4161822694836557E-2</v>
       </c>
       <c r="N19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="O19" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="P19">
         <v>4.7099999999999998E-6</v>
       </c>
       <c r="Q19" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>9.2000000000000003E-4</v>
       </c>
       <c r="R19">
@@ -4042,28 +4041,28 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="W19" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>160.40455673709138</v>
       </c>
       <c r="X19" s="13">
-        <f t="shared" si="19"/>
+        <f t="shared" si="33"/>
         <v>1604.0455673709137</v>
       </c>
       <c r="AA19" s="76">
-        <f t="shared" si="12"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AB19" s="1"/>
       <c r="AC19" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>23</v>
       </c>
       <c r="AD19" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="30"/>
         <v>5.1656176934803615E-5</v>
       </c>
       <c r="AE19" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>22.564923744773303</v>
       </c>
       <c r="AV19" s="66" t="s">
@@ -4077,7 +4076,7 @@
       </c>
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A20" s="99"/>
+      <c r="A20" s="98"/>
       <c r="B20">
         <v>1</v>
       </c>
@@ -4107,30 +4106,30 @@
         <v>4.0322099999999996E-3</v>
       </c>
       <c r="K20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="27"/>
         <v>2.0161049999999999E-5</v>
       </c>
       <c r="L20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="32"/>
         <v>2.0843008232103681</v>
       </c>
       <c r="M20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>20.843008232103678</v>
       </c>
       <c r="N20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="O20" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>17.789161764705881</v>
       </c>
       <c r="P20">
         <v>1.9201E-4</v>
       </c>
       <c r="Q20" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>0.30241574999999998</v>
       </c>
       <c r="R20">
@@ -4149,27 +4148,27 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="W20" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>516.91276575633913</v>
       </c>
       <c r="X20" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="33"/>
         <v>5169.127657563391</v>
       </c>
       <c r="AA20" s="77">
-        <f t="shared" si="12"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AC20" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>75</v>
       </c>
       <c r="AD20" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="30"/>
         <v>6.689085819105817E-3</v>
       </c>
       <c r="AE20" s="60">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>39.719565437732463</v>
       </c>
       <c r="AV20" s="66"/>
@@ -4187,13 +4186,13 @@
       <c r="X21" s="48"/>
       <c r="Z21" s="1"/>
       <c r="AN21" s="66"/>
-      <c r="AO21" s="96"/>
+      <c r="AO21" s="95"/>
       <c r="AP21" s="66"/>
       <c r="AQ21" s="66"/>
       <c r="AR21" s="66"/>
       <c r="AS21" s="66"/>
-      <c r="AT21" s="83"/>
-      <c r="AU21" s="83"/>
+      <c r="AT21" s="82"/>
+      <c r="AU21" s="82"/>
       <c r="AV21" s="7" t="s">
         <v>49</v>
       </c>
@@ -4215,13 +4214,13 @@
         <v>3</v>
       </c>
       <c r="AN22" s="66"/>
-      <c r="AO22" s="96"/>
+      <c r="AO22" s="95"/>
       <c r="AP22" s="66"/>
       <c r="AQ22" s="66"/>
       <c r="AR22" s="66"/>
       <c r="AS22" s="66"/>
-      <c r="AT22" s="83"/>
-      <c r="AU22" s="83"/>
+      <c r="AT22" s="82"/>
+      <c r="AU22" s="82"/>
       <c r="AV22" s="7" t="s">
         <v>50</v>
       </c>
@@ -4242,13 +4241,13 @@
         <v>120</v>
       </c>
       <c r="AN23" s="66"/>
-      <c r="AO23" s="96"/>
+      <c r="AO23" s="95"/>
       <c r="AP23" s="66"/>
       <c r="AQ23" s="66"/>
       <c r="AR23" s="66"/>
       <c r="AS23" s="66"/>
-      <c r="AT23" s="83"/>
-      <c r="AU23" s="83"/>
+      <c r="AT23" s="82"/>
+      <c r="AU23" s="82"/>
       <c r="AV23" s="7" t="s">
         <v>60</v>
       </c>
@@ -4277,7 +4276,7 @@
       </c>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A25" s="99" t="s">
+      <c r="A25" s="98" t="s">
         <v>72</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -4333,7 +4332,7 @@
       </c>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A26" s="99"/>
+      <c r="A26" s="98"/>
       <c r="B26">
         <v>1</v>
       </c>
@@ -4382,7 +4381,7 @@
       <c r="AV26" s="7"/>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A27" s="99"/>
+      <c r="A27" s="98"/>
       <c r="B27">
         <v>1</v>
       </c>
@@ -4437,7 +4436,7 @@
       <c r="Q27" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="R27" s="100" t="s">
+      <c r="R27" s="99" t="s">
         <v>46</v>
       </c>
       <c r="S27" s="7" t="s">
@@ -4491,7 +4490,7 @@
       <c r="Q28" s="14">
         <v>1.2</v>
       </c>
-      <c r="R28" s="100"/>
+      <c r="R28" s="99"/>
       <c r="S28" s="7" t="s">
         <v>48</v>
       </c>
@@ -4513,7 +4512,7 @@
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="F29" s="1"/>
-      <c r="R29" s="100"/>
+      <c r="R29" s="99"/>
       <c r="S29" s="7" t="s">
         <v>49</v>
       </c>
@@ -4551,7 +4550,7 @@
         <f>K27+SUM(J15:J20)+SUM(AK5:AK12)</f>
         <v>5.3968168854811233E-2</v>
       </c>
-      <c r="R30" s="100"/>
+      <c r="R30" s="99"/>
       <c r="S30" s="7" t="s">
         <v>50</v>
       </c>
@@ -4595,7 +4594,7 @@
         <f>( 0.000001*14) / 0.151</f>
         <v>9.2715231788079476E-5</v>
       </c>
-      <c r="R31" s="100"/>
+      <c r="R31" s="99"/>
       <c r="S31" s="7" t="s">
         <v>51</v>
       </c>
@@ -4642,7 +4641,7 @@
         <f>E26*E31+F26*F31</f>
         <v>0</v>
       </c>
-      <c r="R32" s="100"/>
+      <c r="R32" s="99"/>
       <c r="S32" s="9" t="s">
         <v>52</v>
       </c>
@@ -4681,7 +4680,7 @@
       </c>
     </row>
     <row r="35" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="101" t="s">
+      <c r="A35" s="100" t="s">
         <v>152</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -4730,7 +4729,7 @@
       <c r="Q35" s="27"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A36" s="101"/>
+      <c r="A36" s="100"/>
       <c r="B36">
         <v>1</v>
       </c>
@@ -4881,11 +4880,11 @@
       <c r="E1" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="W1" s="93" t="s">
-        <v>172</v>
-      </c>
-      <c r="X1" s="94" t="s">
-        <v>173</v>
+      <c r="W1" s="92" t="s">
+        <v>170</v>
+      </c>
+      <c r="X1" s="93" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:55" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4900,15 +4899,15 @@
         <f xml:space="preserve"> 76.1/12*24*3600</f>
         <v>547920</v>
       </c>
-      <c r="W2" s="95">
+      <c r="W2" s="94">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="X2" s="95">
+      <c r="X2" s="94">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="4" spans="1:55" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="98" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -4975,7 +4974,7 @@
         <v>13</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="X4" s="5" t="s">
         <v>14</v>
@@ -5028,8 +5027,8 @@
       <c r="AN4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AO4" s="97" t="s">
-        <v>179</v>
+      <c r="AO4" s="96" t="s">
+        <v>177</v>
       </c>
       <c r="AP4" s="12" t="s">
         <v>77</v>
@@ -5047,10 +5046,10 @@
         <v>24</v>
       </c>
       <c r="AU4" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="AV4" s="86" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="AV4" s="85" t="s">
+        <v>160</v>
       </c>
       <c r="AW4" s="6" t="s">
         <v>63</v>
@@ -5073,7 +5072,7 @@
       </c>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A5" s="99"/>
+      <c r="A5" s="98"/>
       <c r="B5">
         <v>1</v>
       </c>
@@ -5167,19 +5166,19 @@
         <v>33</v>
       </c>
       <c r="AE5" s="1">
-        <f>AK5*$AQ$15</f>
+        <f t="shared" ref="AE5:AE12" si="0">AK5*$AQ$15</f>
         <v>9.0399389163552328</v>
       </c>
       <c r="AF5" s="1">
-        <f>AK5*$AS5</f>
+        <f t="shared" ref="AF5:AF12" si="1">AK5*$AS5</f>
         <v>1.0111902874411887</v>
       </c>
       <c r="AG5" s="24">
-        <f>AK5*$AV5</f>
+        <f t="shared" ref="AG5:AG12" si="2">AK5*$AV5</f>
         <v>9.0399389163552328</v>
       </c>
       <c r="AH5" s="28">
-        <f>AK5*$AT5</f>
+        <f t="shared" ref="AH5:AH12" si="3">AK5*$AT5</f>
         <v>10.111902874411886</v>
       </c>
       <c r="AI5" s="1">
@@ -5210,29 +5209,29 @@
         <v>1800</v>
       </c>
       <c r="AP5" s="58">
-        <f>AK5+AE5*$E$31+AF5*$F$31+AH5*$J$31</f>
+        <f t="shared" ref="AP5:AP12" si="4">AK5+AE5*$E$31+AF5*$F$31+AH5*$J$31</f>
         <v>3.3497283868557494E-3</v>
       </c>
       <c r="AQ5" s="59">
-        <f>(1-AK5/AP5)*100</f>
+        <f t="shared" ref="AQ5:AQ12" si="5">(1-AK5/AP5)*100</f>
         <v>38.829284515098252</v>
       </c>
       <c r="AR5" s="13">
         <v>4.5999999999999996</v>
       </c>
       <c r="AS5" s="13">
-        <f>(($AR5/100)*(1+($AQ$15+$AV5)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR5/100))</f>
+        <f t="shared" ref="AS5:AS12" si="6">(($AR5/100)*(1+($AQ$15+$AV5)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR5/100))</f>
         <v>493.49156696102204</v>
       </c>
       <c r="AT5" s="13">
-        <f>$AS5/$X$23</f>
+        <f t="shared" ref="AT5:AT12" si="7">$AS5/$X$23</f>
         <v>4934.91566961022</v>
       </c>
       <c r="AU5" s="13">
         <v>10</v>
       </c>
       <c r="AV5" s="71">
-        <f>$AU5/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" ref="AV5:AV12" si="8">$AU5/100/(1-$X$33)*$X$32*10^6/$X$30</f>
         <v>4411.7647058823532</v>
       </c>
       <c r="AW5" s="7">
@@ -5243,7 +5242,7 @@
         <v>9.1058115591388438E-4</v>
       </c>
       <c r="AY5" s="7">
-        <f>J5*Z5</f>
+        <f t="shared" ref="AY5:AY12" si="9">J5*Z5</f>
         <v>2.6054999999999997E-3</v>
       </c>
       <c r="AZ5" s="8">
@@ -5251,17 +5250,17 @@
         <v>2.0477283347659267E-3</v>
       </c>
       <c r="BA5" s="8">
-        <f>$T$27+$T$28*$T$30*(L5)^$T$29</f>
+        <f t="shared" ref="BA5:BA12" si="10">$T$27+$T$28*$T$30*(L5)^$T$29</f>
         <v>4.0277279389003447E-3</v>
       </c>
       <c r="BB5" s="7"/>
       <c r="BC5" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M5)^$AW$21</f>
+        <f t="shared" ref="BC5:BC12" si="11">$AX$20*$AW$22*$AW$24*(M5)^$AW$21</f>
         <v>1.3244862745926676E-6</v>
       </c>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A6" s="99"/>
+      <c r="A6" s="98"/>
       <c r="B6">
         <v>1</v>
       </c>
@@ -5272,7 +5271,7 @@
         <v>4</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E11" si="0">(10-D6)*$E$2</f>
+        <f t="shared" ref="E6:E11" si="12">(10-D6)*$E$2</f>
         <v>3287520</v>
       </c>
       <c r="F6">
@@ -5292,7 +5291,7 @@
         <v>2.894E-2</v>
       </c>
       <c r="K6" s="38">
-        <f t="shared" ref="K6:K12" si="1">J6-M6</f>
+        <f t="shared" ref="K6:K12" si="13">J6-M6</f>
         <v>2.8930000000000001E-2</v>
       </c>
       <c r="L6" s="38">
@@ -5329,7 +5328,7 @@
         <v>3.3993521965748258E-2</v>
       </c>
       <c r="W6" s="1">
-        <f t="shared" ref="W6:W12" si="2">$W$2*EXP($X$2*E6)</f>
+        <f t="shared" ref="W6:W12" si="14">$W$2*EXP($X$2*E6)</f>
         <v>2.6776375833009532E-5</v>
       </c>
       <c r="X6" t="s">
@@ -5354,19 +5353,19 @@
         <v>33</v>
       </c>
       <c r="AE6" s="1">
-        <f>AK6*$AQ$15</f>
+        <f t="shared" si="0"/>
         <v>3.5017162544188412</v>
       </c>
       <c r="AF6" s="1">
-        <f>AK6*$AS6</f>
+        <f t="shared" si="1"/>
         <v>0.65956141271581703</v>
       </c>
       <c r="AG6" s="24">
-        <f>AK6*$AV6</f>
+        <f t="shared" si="2"/>
         <v>1.7508581272094206</v>
       </c>
       <c r="AH6" s="28">
-        <f>AK6*$AT6</f>
+        <f t="shared" si="3"/>
         <v>6.5956141271581705</v>
       </c>
       <c r="AI6" s="1">
@@ -5378,48 +5377,48 @@
         <v>1.6879744031468265E-7</v>
       </c>
       <c r="AK6">
-        <f t="shared" ref="AK6:AK12" si="3">AI6+AJ6</f>
+        <f t="shared" ref="AK6:AK12" si="15">AI6+AJ6</f>
         <v>7.9372235100160394E-4</v>
       </c>
       <c r="AL6">
-        <f t="shared" ref="AL6:AM12" si="4">AI6*0.005</f>
+        <f t="shared" ref="AL6:AM12" si="16">AI6*0.005</f>
         <v>3.9677677678064465E-6</v>
       </c>
       <c r="AM6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>8.4398720157341326E-10</v>
       </c>
       <c r="AN6">
-        <f t="shared" ref="AN6:AN12" si="5">AL6+AM6</f>
+        <f t="shared" ref="AN6:AN12" si="17">AL6+AM6</f>
         <v>3.9686117550080197E-6</v>
       </c>
       <c r="AO6" s="1">
         <v>1800</v>
       </c>
       <c r="AP6" s="58">
-        <f>AK6+AE6*$E$31+AF6*$F$31+AH6*$J$31</f>
+        <f t="shared" si="4"/>
         <v>1.5736842407450208E-3</v>
       </c>
       <c r="AQ6" s="59">
-        <f>(1-AK6/AP6)*100</f>
+        <f t="shared" si="5"/>
         <v>49.562794717583479</v>
       </c>
       <c r="AR6" s="13">
         <v>6.5</v>
       </c>
       <c r="AS6" s="13">
-        <f>(($AR6/100)*(1+($AQ$15+$AV6)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR6/100))</f>
+        <f t="shared" si="6"/>
         <v>830.97245766546928</v>
       </c>
       <c r="AT6" s="13">
-        <f>$AS6/$X$23</f>
+        <f t="shared" si="7"/>
         <v>8309.724576654693</v>
       </c>
       <c r="AU6" s="13">
         <v>5</v>
       </c>
       <c r="AV6" s="71">
-        <f>$AU6/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>2205.8823529411766</v>
       </c>
       <c r="AW6" s="7">
@@ -5430,7 +5429,7 @@
         <v>9.1017858127080242E-4</v>
       </c>
       <c r="AY6" s="7" t="e">
-        <f>J6*Z6</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ6" s="8" t="e">
@@ -5438,17 +5437,17 @@
         <v>#VALUE!</v>
       </c>
       <c r="BA6" s="8">
-        <f>$T$27+$T$28*$T$30*(L6)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>7.9355355356128927E-4</v>
       </c>
       <c r="BB6" s="7"/>
       <c r="BC6" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M6)^$AW$21</f>
+        <f t="shared" si="11"/>
         <v>1.6879744031468265E-7</v>
       </c>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A7" s="99"/>
+      <c r="A7" s="98"/>
       <c r="B7">
         <v>1</v>
       </c>
@@ -5459,7 +5458,7 @@
         <v>5</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>2739600</v>
       </c>
       <c r="F7">
@@ -5479,7 +5478,7 @@
         <v>2.894E-2</v>
       </c>
       <c r="K7" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
       <c r="L7" s="38">
@@ -5516,7 +5515,7 @@
         <v>32</v>
       </c>
       <c r="W7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1.5480791541095022E-5</v>
       </c>
       <c r="X7" t="s">
@@ -5541,19 +5540,19 @@
         <v>33</v>
       </c>
       <c r="AE7" s="1">
-        <f>AK7*$AQ$15</f>
+        <f t="shared" si="0"/>
         <v>0.13143561599020981</v>
       </c>
       <c r="AF7" s="1">
-        <f>AK7*$AS7</f>
+        <f t="shared" si="1"/>
         <v>5.4184269937105296E-2</v>
       </c>
       <c r="AG7" s="24">
-        <f>AK7*$AV7</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH7" s="28">
-        <f>AK7*$AT7</f>
+        <f t="shared" si="3"/>
         <v>0.54184269937105289</v>
       </c>
       <c r="AI7" s="1">
@@ -5564,75 +5563,75 @@
         <v>0</v>
       </c>
       <c r="AK7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>2.9792072957780891E-5</v>
       </c>
       <c r="AL7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>1.4896036478890447E-7</v>
       </c>
       <c r="AM7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AN7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="17"/>
         <v>1.4896036478890447E-7</v>
       </c>
       <c r="AO7" s="1">
         <v>1800</v>
       </c>
       <c r="AP7" s="58">
-        <f>AK7+AE7*$E$31+AF7*$F$31+AH7*$J$31</f>
+        <f t="shared" si="4"/>
         <v>8.9403557211611783E-5</v>
       </c>
       <c r="AQ7" s="59">
-        <f>(1-AK7/AP7)*100</f>
+        <f t="shared" si="5"/>
         <v>66.676859526668281</v>
       </c>
       <c r="AR7" s="13">
         <v>9.5</v>
       </c>
       <c r="AS7" s="13">
-        <f>(($AR7/100)*(1+($AQ$15+$AV7)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR7/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AT7" s="13">
-        <f>$AS7/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AU7" s="13">
         <v>0</v>
       </c>
       <c r="AV7" s="71">
-        <f>$AU7/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW7" s="7"/>
       <c r="AX7" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T7*$T$32)^$T$29</f>
+        <f t="shared" ref="AX7:AX12" si="18">$T$27+$T$28*$T$30*(T7*$T$32)^$T$29</f>
         <v>#VALUE!</v>
       </c>
       <c r="AY7" s="7" t="e">
-        <f>J7*Z7</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ7" s="8" t="e">
-        <f>AX7+((AY7-AX7)/$T$31)*F7</f>
+        <f t="shared" ref="AZ7:AZ12" si="19">AX7+((AY7-AX7)/$T$31)*F7</f>
         <v>#VALUE!</v>
       </c>
       <c r="BA7" s="8">
-        <f>$T$27+$T$28*$T$30*(L7)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>2.9792072957780891E-5</v>
       </c>
       <c r="BB7" s="7"/>
       <c r="BC7" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M7)^$AW$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A8" s="99"/>
+      <c r="A8" s="98"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -5643,7 +5642,7 @@
         <v>6</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>2191680</v>
       </c>
       <c r="F8">
@@ -5659,11 +5658,11 @@
         <v>33</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:J12" si="6">J7-M8</f>
+        <f t="shared" ref="J8:J12" si="20">J7-M8</f>
         <v>2.894E-2</v>
       </c>
       <c r="K8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
       <c r="L8" s="38">
@@ -5700,7 +5699,7 @@
         <v>32</v>
       </c>
       <c r="W8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>8.9502368891684043E-6</v>
       </c>
       <c r="X8" t="s">
@@ -5725,98 +5724,98 @@
         <v>33</v>
       </c>
       <c r="AE8" s="1">
-        <f>AK8*$AQ$15</f>
+        <f t="shared" si="0"/>
         <v>3.5630437425207336E-2</v>
       </c>
       <c r="AF8" s="1">
-        <f>AK8*$AS8</f>
+        <f t="shared" si="1"/>
         <v>1.4688630816538933E-2</v>
       </c>
       <c r="AG8" s="24">
-        <f>AK8*$AV8</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH8" s="28">
-        <f>AK8*$AT8</f>
+        <f t="shared" si="3"/>
         <v>0.14688630816538931</v>
       </c>
       <c r="AI8" s="1">
-        <f t="shared" ref="AI8:AI12" si="7">BA8</f>
+        <f t="shared" ref="AI8:AI12" si="21">BA8</f>
         <v>8.076232483046996E-6</v>
       </c>
       <c r="AJ8" s="1">
         <v>0</v>
       </c>
       <c r="AK8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>8.076232483046996E-6</v>
       </c>
       <c r="AL8">
+        <f t="shared" si="16"/>
+        <v>4.0381162415234981E-8</v>
+      </c>
+      <c r="AM8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <f t="shared" si="17"/>
+        <v>4.0381162415234981E-8</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP8" s="58">
         <f t="shared" si="4"/>
-        <v>4.0381162415234981E-8</v>
-      </c>
-      <c r="AM8">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AN8">
+        <v>2.4236108506970847E-5</v>
+      </c>
+      <c r="AQ8" s="59">
         <f t="shared" si="5"/>
-        <v>4.0381162415234981E-8</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP8" s="58">
-        <f>AK8+AE8*$E$31+AF8*$F$31+AH8*$J$31</f>
-        <v>2.4236108506970847E-5</v>
-      </c>
-      <c r="AQ8" s="59">
-        <f>(1-AK8/AP8)*100</f>
         <v>66.676859526668281</v>
       </c>
       <c r="AR8" s="13">
         <v>9.5</v>
       </c>
       <c r="AS8" s="13">
-        <f>(($AR8/100)*(1+($AQ$15+$AV8)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR8/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AT8" s="13">
-        <f>$AS8/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AU8" s="13">
         <v>0</v>
       </c>
       <c r="AV8" s="71">
-        <f>$AU8/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW8" s="7"/>
       <c r="AX8" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T8*$T$32)^$T$29</f>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="AY8" s="7" t="e">
-        <f>J8*Z8</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ8" s="8" t="e">
-        <f>AX8+((AY8-AX8)/$T$31)*F8</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BA8" s="8">
-        <f>$T$27+$T$28*$T$30*(L8)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>8.076232483046996E-6</v>
       </c>
       <c r="BB8" s="7"/>
       <c r="BC8" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M8)^$AW$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A9" s="99"/>
+      <c r="A9" s="98"/>
       <c r="B9">
         <v>1</v>
       </c>
@@ -5827,7 +5826,7 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>1643760</v>
       </c>
       <c r="F9">
@@ -5843,11 +5842,11 @@
         <v>33</v>
       </c>
       <c r="J9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="20"/>
         <v>2.894E-2</v>
       </c>
       <c r="K9" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
       <c r="L9" s="38">
@@ -5884,7 +5883,7 @@
         <v>32</v>
       </c>
       <c r="W9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>5.1745894361784425E-6</v>
       </c>
       <c r="X9" t="s">
@@ -5909,98 +5908,98 @@
         <v>33</v>
       </c>
       <c r="AE9" s="1">
-        <f>AK9*$AQ$15</f>
+        <f t="shared" si="0"/>
         <v>1.2193691971899337E-2</v>
       </c>
       <c r="AF9" s="1">
-        <f>AK9*$AS9</f>
+        <f t="shared" si="1"/>
         <v>5.0268436934515614E-3</v>
       </c>
       <c r="AG9" s="24">
-        <f>AK9*$AV9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH9" s="28">
-        <f>AK9*$AT9</f>
+        <f t="shared" si="3"/>
         <v>5.026843693451561E-2</v>
       </c>
       <c r="AI9" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>2.7639035136305163E-6</v>
       </c>
       <c r="AJ9" s="1">
         <v>0</v>
       </c>
       <c r="AK9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>2.7639035136305163E-6</v>
       </c>
       <c r="AL9">
+        <f t="shared" si="16"/>
+        <v>1.3819517568152583E-8</v>
+      </c>
+      <c r="AM9">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <f t="shared" si="17"/>
+        <v>1.3819517568152583E-8</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP9" s="58">
         <f t="shared" si="4"/>
-        <v>1.3819517568152583E-8</v>
-      </c>
-      <c r="AM9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AN9">
+        <v>8.294246803786242E-6</v>
+      </c>
+      <c r="AQ9" s="59">
         <f t="shared" si="5"/>
-        <v>1.3819517568152583E-8</v>
-      </c>
-      <c r="AO9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP9" s="58">
-        <f>AK9+AE9*$E$31+AF9*$F$31+AH9*$J$31</f>
-        <v>8.294246803786242E-6</v>
-      </c>
-      <c r="AQ9" s="59">
-        <f>(1-AK9/AP9)*100</f>
         <v>66.676859526668281</v>
       </c>
       <c r="AR9" s="13">
         <v>9.5</v>
       </c>
       <c r="AS9" s="13">
-        <f>(($AR9/100)*(1+($AQ$15+$AV9)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR9/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AT9" s="13">
-        <f>$AS9/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AU9" s="13">
         <v>0</v>
       </c>
       <c r="AV9" s="71">
-        <f>$AU9/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW9" s="7"/>
       <c r="AX9" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T9*$T$32)^$T$29</f>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="AY9" s="7" t="e">
-        <f>J9*Z9</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ9" s="8" t="e">
-        <f>AX9+((AY9-AX9)/$T$31)*F9</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BA9" s="8">
-        <f>$T$27+$T$28*$T$30*(L9)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>2.7639035136305163E-6</v>
       </c>
       <c r="BB9" s="7"/>
       <c r="BC9" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M9)^$AW$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A10" s="99"/>
+      <c r="A10" s="98"/>
       <c r="B10">
         <v>1</v>
       </c>
@@ -6011,7 +6010,7 @@
         <v>8</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>1095840</v>
       </c>
       <c r="F10">
@@ -6027,11 +6026,11 @@
         <v>33</v>
       </c>
       <c r="J10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="20"/>
         <v>2.894E-2</v>
       </c>
       <c r="K10" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
       <c r="L10" s="38">
@@ -6068,7 +6067,7 @@
         <v>32</v>
       </c>
       <c r="W10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>2.9916946517264094E-6</v>
       </c>
       <c r="X10" t="s">
@@ -6093,98 +6092,98 @@
         <v>33</v>
       </c>
       <c r="AE10" s="1">
-        <f>AK10*$AQ$15</f>
+        <f t="shared" si="0"/>
         <v>5.2963394285683064E-3</v>
       </c>
       <c r="AF10" s="1">
-        <f>AK10*$AS10</f>
+        <f t="shared" si="1"/>
         <v>2.1834134006527969E-3</v>
       </c>
       <c r="AG10" s="24">
-        <f>AK10*$AV10</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH10" s="28">
-        <f>AK10*$AT10</f>
+        <f t="shared" si="3"/>
         <v>2.1834134006527964E-2</v>
       </c>
       <c r="AI10" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>1.2005036038088161E-6</v>
       </c>
       <c r="AJ10" s="1">
         <v>0</v>
       </c>
       <c r="AK10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>1.2005036038088161E-6</v>
       </c>
       <c r="AL10">
+        <f t="shared" si="16"/>
+        <v>6.0025180190440811E-9</v>
+      </c>
+      <c r="AM10">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <f t="shared" si="17"/>
+        <v>6.0025180190440811E-9</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP10" s="58">
         <f t="shared" si="4"/>
-        <v>6.0025180190440811E-9</v>
-      </c>
-      <c r="AM10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AN10">
+        <v>3.6026124391534188E-6</v>
+      </c>
+      <c r="AQ10" s="59">
         <f t="shared" si="5"/>
-        <v>6.0025180190440811E-9</v>
-      </c>
-      <c r="AO10" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP10" s="58">
-        <f>AK10+AE10*$E$31+AF10*$F$31+AH10*$J$31</f>
-        <v>3.6026124391534188E-6</v>
-      </c>
-      <c r="AQ10" s="59">
-        <f>(1-AK10/AP10)*100</f>
         <v>66.676859526668281</v>
       </c>
       <c r="AR10" s="13">
         <v>9.5</v>
       </c>
       <c r="AS10" s="13">
-        <f>(($AR10/100)*(1+($AQ$15+$AV10)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR10/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AT10" s="13">
-        <f>$AS10/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AU10" s="13">
         <v>0</v>
       </c>
       <c r="AV10" s="71">
-        <f>$AU10/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW10" s="7"/>
       <c r="AX10" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T10*$T$32)^$T$29</f>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="AY10" s="7" t="e">
-        <f>J10*Z10</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ10" s="8" t="e">
-        <f>AX10+((AY10-AX10)/$T$31)*F10</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BA10" s="8">
-        <f>$T$27+$T$28*$T$30*(L10)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>1.2005036038088161E-6</v>
       </c>
       <c r="BB10" s="7"/>
       <c r="BC10" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M10)^$AW$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A11" s="99"/>
+      <c r="A11" s="98"/>
       <c r="B11">
         <v>1</v>
       </c>
@@ -6195,7 +6194,7 @@
         <v>9</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="12"/>
         <v>547920</v>
       </c>
       <c r="F11">
@@ -6211,11 +6210,11 @@
         <v>33</v>
       </c>
       <c r="J11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="20"/>
         <v>2.894E-2</v>
       </c>
       <c r="K11" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
       <c r="L11" s="39">
@@ -6252,7 +6251,7 @@
         <v>32</v>
       </c>
       <c r="W11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1.7296515983649451E-6</v>
       </c>
       <c r="X11" t="s">
@@ -6277,98 +6276,98 @@
         <v>33</v>
       </c>
       <c r="AE11" s="1">
-        <f>AK11*$AQ$15</f>
+        <f t="shared" si="0"/>
         <v>1.9146799290632522E-3</v>
       </c>
       <c r="AF11" s="1">
-        <f>AK11*$AS11</f>
+        <f t="shared" si="1"/>
         <v>7.8932588657893549E-4</v>
       </c>
       <c r="AG11" s="24">
-        <f>AK11*$AV11</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH11" s="28">
-        <f>AK11*$AT11</f>
+        <f t="shared" si="3"/>
         <v>7.8932588657893536E-3</v>
       </c>
       <c r="AI11" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>4.3399411725433714E-7</v>
       </c>
       <c r="AJ11" s="1">
         <v>0</v>
       </c>
       <c r="AK11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>4.3399411725433714E-7</v>
       </c>
       <c r="AL11">
+        <f t="shared" si="16"/>
+        <v>2.1699705862716857E-9</v>
+      </c>
+      <c r="AM11">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <f t="shared" si="17"/>
+        <v>2.1699705862716857E-9</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP11" s="58">
         <f t="shared" si="4"/>
-        <v>2.1699705862716857E-9</v>
-      </c>
-      <c r="AM11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AN11">
+        <v>1.3023806012571343E-6</v>
+      </c>
+      <c r="AQ11" s="59">
         <f t="shared" si="5"/>
-        <v>2.1699705862716857E-9</v>
-      </c>
-      <c r="AO11" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP11" s="58">
-        <f>AK11+AE11*$E$31+AF11*$F$31+AH11*$J$31</f>
-        <v>1.3023806012571343E-6</v>
-      </c>
-      <c r="AQ11" s="59">
-        <f>(1-AK11/AP11)*100</f>
         <v>66.676859526668281</v>
       </c>
       <c r="AR11" s="13">
         <v>9.5</v>
       </c>
       <c r="AS11" s="13">
-        <f>(($AR11/100)*(1+($AQ$15+$AV11)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR11/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AT11" s="13">
-        <f>$AS11/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AU11" s="13">
         <v>0</v>
       </c>
       <c r="AV11" s="71">
-        <f>$AU11/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW11" s="7"/>
       <c r="AX11" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T11*$T$32)^$T$29</f>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="AY11" s="7" t="e">
-        <f>J11*Z11</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ11" s="8" t="e">
-        <f>AX11+((AY11-AX11)/$T$31)*F11</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BA11" s="8">
-        <f>$T$27+$T$28*$T$30*(L11)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>4.3399411725433714E-7</v>
       </c>
       <c r="BB11" s="7"/>
       <c r="BC11" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M11)^$AW$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A12" s="99"/>
+      <c r="A12" s="98"/>
       <c r="B12">
         <v>1</v>
       </c>
@@ -6395,11 +6394,11 @@
         <v>33</v>
       </c>
       <c r="J12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="20"/>
         <v>2.894E-2</v>
       </c>
       <c r="K12" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.894E-2</v>
       </c>
       <c r="L12" s="39">
@@ -6436,7 +6435,7 @@
         <v>32</v>
       </c>
       <c r="W12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="X12" t="s">
@@ -6461,93 +6460,93 @@
         <v>33</v>
       </c>
       <c r="AE12" s="1">
-        <f>AK12*$AQ$15</f>
+        <f t="shared" si="0"/>
         <v>1.2855761246405892E-3</v>
       </c>
       <c r="AF12" s="1">
-        <f>AK12*$AS12</f>
+        <f t="shared" si="1"/>
         <v>5.2997814357572592E-4</v>
       </c>
       <c r="AG12" s="24">
-        <f>AK12*$AV12</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH12" s="28">
-        <f>AK12*$AT12</f>
+        <f t="shared" si="3"/>
         <v>5.2997814357572583E-3</v>
       </c>
       <c r="AI12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="21"/>
         <v>2.9139725491853351E-7</v>
       </c>
       <c r="AJ12" s="1">
         <v>0</v>
       </c>
       <c r="AK12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>2.9139725491853351E-7</v>
       </c>
       <c r="AL12">
+        <f t="shared" si="16"/>
+        <v>1.4569862745926675E-9</v>
+      </c>
+      <c r="AM12">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AN12">
+        <f t="shared" si="17"/>
+        <v>1.4569862745926675E-9</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP12" s="61">
         <f t="shared" si="4"/>
-        <v>1.4569862745926675E-9</v>
-      </c>
-      <c r="AM12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AN12">
+        <v>8.7445916195004701E-7</v>
+      </c>
+      <c r="AQ12" s="60">
         <f t="shared" si="5"/>
-        <v>1.4569862745926675E-9</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP12" s="61">
-        <f>AK12+AE12*$E$31+AF12*$F$31+AH12*$J$31</f>
-        <v>8.7445916195004701E-7</v>
-      </c>
-      <c r="AQ12" s="60">
-        <f>(1-AK12/AP12)*100</f>
         <v>66.676859526668281</v>
       </c>
       <c r="AR12" s="14">
         <v>9.5</v>
       </c>
       <c r="AS12" s="13">
-        <f>(($AR12/100)*(1+($AQ$15+$AV12)*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$AR12/100))</f>
+        <f t="shared" si="6"/>
         <v>1818.7478935719314</v>
       </c>
       <c r="AT12" s="14">
-        <f>$AS12/$X$23</f>
+        <f t="shared" si="7"/>
         <v>18187.478935719311</v>
       </c>
       <c r="AU12" s="14">
         <v>0</v>
       </c>
       <c r="AV12" s="71">
-        <f>$AU12/100/(1-$X$33)*$X$32*10^6/$X$30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW12" s="7"/>
       <c r="AX12" s="8" t="e">
-        <f>$T$27+$T$28*$T$30*(T12*$T$32)^$T$29</f>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="AY12" s="7" t="e">
-        <f>J12*Z12</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ12" s="8" t="e">
-        <f>AX12+((AY12-AX12)/$T$31)*F12</f>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="BA12" s="8">
-        <f>$T$27+$T$28*$T$30*(L12)^$T$29</f>
+        <f t="shared" si="10"/>
         <v>2.9139725491853351E-7</v>
       </c>
       <c r="BB12" s="7"/>
       <c r="BC12" s="7">
-        <f>$AX$20*$AW$22*$AW$24*(M12)^$AW$21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -6564,7 +6563,7 @@
       <c r="AF13" s="1"/>
     </row>
     <row r="14" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="99" t="s">
+      <c r="A14" s="98" t="s">
         <v>71</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -6665,7 +6664,7 @@
       <c r="AU14" s="40"/>
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A15" s="99"/>
+      <c r="A15" s="98"/>
       <c r="B15">
         <v>1</v>
       </c>
@@ -6704,15 +6703,15 @@
         <v>1.6239747221660625</v>
       </c>
       <c r="M15">
-        <f t="shared" ref="M15:M20" si="8">J15*$X15</f>
+        <f t="shared" ref="M15:M20" si="22">J15*$X15</f>
         <v>16.239747221660625</v>
       </c>
       <c r="N15">
-        <f t="shared" ref="N15:N20" si="9">AA15*$J15</f>
+        <f t="shared" ref="N15:N20" si="23">AA15*$J15</f>
         <v>0</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" ref="O15:O20" si="10">J15*$AB$16</f>
+        <f t="shared" ref="O15:O20" si="24">J15*$AB$16</f>
         <v>18.09675</v>
       </c>
       <c r="P15">
@@ -6738,7 +6737,7 @@
         <v>4.3</v>
       </c>
       <c r="W15" s="13">
-        <f t="shared" ref="W15:W20" si="11">(($V15/100)*(1+$AB$16*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$V15/100))</f>
+        <f t="shared" ref="W15:W20" si="25">(($V15/100)*(1+$AB$16*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$V15/100))</f>
         <v>395.90503059926971</v>
       </c>
       <c r="X15" s="13">
@@ -6752,7 +6751,7 @@
         <v>27</v>
       </c>
       <c r="AA15" s="76">
-        <f t="shared" ref="AA15:AA20" si="12">IF(F15="HiddenElement",$AA$22/100/(1-$X$33)*$X$32*10^6/$X$30,0)</f>
+        <f t="shared" ref="AA15:AA20" si="26">IF(F15="HiddenElement",$AA$22/100/(1-$X$33)*$X$32*10^6/$X$30,0)</f>
         <v>0</v>
       </c>
       <c r="AB15" s="75" t="s">
@@ -6784,11 +6783,11 @@
         <f>AR15+AQ15</f>
         <v>8823.5294117647063</v>
       </c>
-      <c r="AT15" s="84"/>
-      <c r="AU15" s="84"/>
+      <c r="AT15" s="83"/>
+      <c r="AU15" s="83"/>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A16" s="99"/>
+      <c r="A16" s="98"/>
       <c r="B16">
         <v>1</v>
       </c>
@@ -6819,7 +6818,7 @@
         <v>1.7099999999999999E-3</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K16:K20" si="13">J16*0.005</f>
+        <f t="shared" ref="K16:K20" si="27">J16*0.005</f>
         <v>8.5499999999999995E-6</v>
       </c>
       <c r="L16">
@@ -6827,22 +6826,22 @@
         <v>0.19277131424832977</v>
       </c>
       <c r="M16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>1.9277131424832974</v>
       </c>
       <c r="N16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="O16" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>7.5441176470588234</v>
       </c>
       <c r="P16">
         <v>2.6861000000000002E-4</v>
       </c>
       <c r="Q16" s="1">
-        <f t="shared" ref="Q16:Q20" si="14">J16*$AC16</f>
+        <f t="shared" ref="Q16:Q20" si="28">J16*$AC16</f>
         <v>2.7359999999999999E-2</v>
       </c>
       <c r="R16">
@@ -6862,7 +6861,7 @@
         <v>1.8</v>
       </c>
       <c r="W16" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>112.73176271832151</v>
       </c>
       <c r="X16" s="13">
@@ -6876,7 +6875,7 @@
         <v>1</v>
       </c>
       <c r="AA16" s="76">
-        <f t="shared" si="12"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AB16" s="45">
@@ -6884,15 +6883,15 @@
         <v>4411.7647058823532</v>
       </c>
       <c r="AC16" s="13">
-        <f t="shared" ref="AC16:AC20" si="15">ROUND(X16/$AT$6*120,0)</f>
+        <f t="shared" ref="AC16:AC20" si="29">ROUND(X16/$AT$6*120,0)</f>
         <v>16</v>
       </c>
       <c r="AD16" s="13">
-        <f t="shared" ref="AD16:AD20" si="16">J16+L16*$F$31+M16*$J$31+O16*$E$31</f>
+        <f t="shared" ref="AD16:AD20" si="30">J16+L16*$F$31+M16*$J$31+O16*$E$31</f>
         <v>2.1242656885690431E-3</v>
       </c>
       <c r="AE16" s="59">
-        <f t="shared" ref="AE16:AE20" si="17">(1-J16/AD16)*100</f>
+        <f t="shared" ref="AE16:AE20" si="31">(1-J16/AD16)*100</f>
         <v>19.501594871030591</v>
       </c>
       <c r="AF16" s="1"/>
@@ -6909,11 +6908,11 @@
         <f>AR16+AQ16</f>
         <v>20</v>
       </c>
-      <c r="AT16" s="85"/>
-      <c r="AU16" s="85"/>
+      <c r="AT16" s="84"/>
+      <c r="AU16" s="84"/>
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A17" s="99"/>
+      <c r="A17" s="98"/>
       <c r="B17">
         <v>1</v>
       </c>
@@ -6944,23 +6943,23 @@
         <v>5.0624699999999995E-3</v>
       </c>
       <c r="K17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="27"/>
         <v>2.5312349999999998E-5</v>
       </c>
       <c r="L17">
-        <f t="shared" ref="L17:L20" si="18">J17*$W17</f>
+        <f t="shared" ref="L17:L20" si="32">J17*$W17</f>
         <v>2.3758024102824513</v>
       </c>
       <c r="M17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>23.758024102824514</v>
       </c>
       <c r="N17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>22.334426470588234</v>
       </c>
       <c r="P17">
@@ -6986,38 +6985,38 @@
         <v>4.8</v>
       </c>
       <c r="W17" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>469.29708428542818</v>
       </c>
       <c r="X17" s="13">
-        <f t="shared" ref="X17:X20" si="19">$W17/$X$23</f>
+        <f t="shared" ref="X17:X20" si="33">$W17/$X$23</f>
         <v>4692.9708428542817</v>
       </c>
       <c r="Z17" s="24"/>
       <c r="AA17" s="76">
-        <f t="shared" si="12"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AB17" s="42">
         <v>10</v>
       </c>
       <c r="AC17" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>68</v>
       </c>
       <c r="AD17" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="30"/>
         <v>8.1497066913228666E-3</v>
       </c>
       <c r="AE17" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>37.88156811348685</v>
       </c>
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A18" s="99"/>
+      <c r="A18" s="98"/>
       <c r="B18">
         <v>1</v>
       </c>
@@ -7048,30 +7047,30 @@
         <v>2.2800000000000003E-3</v>
       </c>
       <c r="K18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="27"/>
         <v>1.1400000000000003E-5</v>
       </c>
       <c r="L18">
-        <f t="shared" si="18"/>
+        <f t="shared" si="32"/>
         <v>0.36572238936056839</v>
       </c>
       <c r="M18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>3.6572238936056838</v>
       </c>
       <c r="N18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>3.0176470588235293</v>
       </c>
       <c r="O18" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>10.058823529411766</v>
       </c>
       <c r="P18">
         <v>2.4800000000000001E-4</v>
       </c>
       <c r="Q18" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>5.2440000000000007E-2</v>
       </c>
       <c r="R18">
@@ -7091,11 +7090,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="W18" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>160.40455673709138</v>
       </c>
       <c r="X18" s="13">
-        <f t="shared" si="19"/>
+        <f t="shared" si="33"/>
         <v>1604.0455673709137</v>
       </c>
       <c r="AA18" s="76">
@@ -7106,22 +7105,22 @@
         <v>120</v>
       </c>
       <c r="AC18" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>23</v>
       </c>
       <c r="AD18" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="30"/>
         <v>2.9444020852838065E-3</v>
       </c>
       <c r="AE18" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>22.564923744773314</v>
       </c>
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A19" s="99"/>
+      <c r="A19" s="98"/>
       <c r="B19">
         <v>1</v>
       </c>
@@ -7152,30 +7151,30 @@
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="K19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="27"/>
         <v>2.0000000000000002E-7</v>
       </c>
       <c r="L19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="32"/>
         <v>6.4161822694836562E-3</v>
       </c>
       <c r="M19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>6.4161822694836557E-2</v>
       </c>
       <c r="N19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="O19" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="P19">
         <v>4.7099999999999998E-6</v>
       </c>
       <c r="Q19" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>9.2000000000000003E-4</v>
       </c>
       <c r="R19">
@@ -7195,31 +7194,31 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="W19" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>160.40455673709138</v>
       </c>
       <c r="X19" s="13">
-        <f t="shared" si="19"/>
+        <f t="shared" si="33"/>
         <v>1604.0455673709137</v>
       </c>
       <c r="AA19" s="76">
-        <f t="shared" si="12"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AB19" s="1"/>
       <c r="AC19" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>23</v>
       </c>
       <c r="AD19" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="30"/>
         <v>5.1656176934803615E-5</v>
       </c>
       <c r="AE19" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>22.564923744773303</v>
       </c>
-      <c r="AV19" s="98" t="s">
+      <c r="AV19" s="97" t="s">
         <v>57</v>
       </c>
       <c r="AW19" s="7" t="s">
@@ -7230,7 +7229,7 @@
       </c>
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A20" s="99"/>
+      <c r="A20" s="98"/>
       <c r="B20">
         <v>1</v>
       </c>
@@ -7260,30 +7259,30 @@
         <v>4.0322099999999996E-3</v>
       </c>
       <c r="K20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="27"/>
         <v>2.0161049999999999E-5</v>
       </c>
       <c r="L20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="32"/>
         <v>2.0843008232103681</v>
       </c>
       <c r="M20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>20.843008232103678</v>
       </c>
       <c r="N20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="O20" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>17.789161764705881</v>
       </c>
       <c r="P20">
         <v>1.9201E-4</v>
       </c>
       <c r="Q20" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>0.30241574999999998</v>
       </c>
       <c r="R20">
@@ -7302,30 +7301,30 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="W20" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>516.91276575633913</v>
       </c>
       <c r="X20" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="33"/>
         <v>5169.127657563391</v>
       </c>
       <c r="AA20" s="77">
-        <f t="shared" si="12"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AC20" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>75</v>
       </c>
       <c r="AD20" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="30"/>
         <v>6.689085819105817E-3</v>
       </c>
       <c r="AE20" s="60">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>39.719565437732463</v>
       </c>
-      <c r="AV20" s="98"/>
+      <c r="AV20" s="97"/>
       <c r="AW20" s="7" t="s">
         <v>48</v>
       </c>
@@ -7339,14 +7338,14 @@
       <c r="W21" s="15"/>
       <c r="X21" s="48"/>
       <c r="Z21" s="1"/>
-      <c r="AN21" s="98"/>
-      <c r="AO21" s="98"/>
-      <c r="AP21" s="98"/>
-      <c r="AQ21" s="98"/>
-      <c r="AR21" s="98"/>
-      <c r="AS21" s="98"/>
-      <c r="AT21" s="98"/>
-      <c r="AU21" s="98"/>
+      <c r="AN21" s="97"/>
+      <c r="AO21" s="97"/>
+      <c r="AP21" s="97"/>
+      <c r="AQ21" s="97"/>
+      <c r="AR21" s="97"/>
+      <c r="AS21" s="97"/>
+      <c r="AT21" s="97"/>
+      <c r="AU21" s="97"/>
       <c r="AV21" s="7" t="s">
         <v>49</v>
       </c>
@@ -7367,14 +7366,14 @@
       <c r="AA22" s="42">
         <v>3</v>
       </c>
-      <c r="AN22" s="98"/>
-      <c r="AO22" s="98"/>
-      <c r="AP22" s="98"/>
-      <c r="AQ22" s="98"/>
-      <c r="AR22" s="98"/>
-      <c r="AS22" s="98"/>
-      <c r="AT22" s="98"/>
-      <c r="AU22" s="98"/>
+      <c r="AN22" s="97"/>
+      <c r="AO22" s="97"/>
+      <c r="AP22" s="97"/>
+      <c r="AQ22" s="97"/>
+      <c r="AR22" s="97"/>
+      <c r="AS22" s="97"/>
+      <c r="AT22" s="97"/>
+      <c r="AU22" s="97"/>
       <c r="AV22" s="7" t="s">
         <v>50</v>
       </c>
@@ -7394,14 +7393,14 @@
       <c r="AA23" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="AN23" s="98"/>
-      <c r="AO23" s="98"/>
-      <c r="AP23" s="98"/>
-      <c r="AQ23" s="98"/>
-      <c r="AR23" s="98"/>
-      <c r="AS23" s="98"/>
-      <c r="AT23" s="98"/>
-      <c r="AU23" s="98"/>
+      <c r="AN23" s="97"/>
+      <c r="AO23" s="97"/>
+      <c r="AP23" s="97"/>
+      <c r="AQ23" s="97"/>
+      <c r="AR23" s="97"/>
+      <c r="AS23" s="97"/>
+      <c r="AT23" s="97"/>
+      <c r="AU23" s="97"/>
       <c r="AV23" s="7" t="s">
         <v>60</v>
       </c>
@@ -7430,7 +7429,7 @@
       </c>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A25" s="99" t="s">
+      <c r="A25" s="98" t="s">
         <v>72</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -7486,7 +7485,7 @@
       </c>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A26" s="99"/>
+      <c r="A26" s="98"/>
       <c r="B26">
         <v>1</v>
       </c>
@@ -7535,7 +7534,7 @@
       <c r="AV26" s="7"/>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A27" s="99"/>
+      <c r="A27" s="98"/>
       <c r="B27">
         <v>1</v>
       </c>
@@ -7590,7 +7589,7 @@
       <c r="Q27" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="R27" s="100" t="s">
+      <c r="R27" s="99" t="s">
         <v>46</v>
       </c>
       <c r="S27" s="7" t="s">
@@ -7644,7 +7643,7 @@
       <c r="Q28" s="14">
         <v>1.2</v>
       </c>
-      <c r="R28" s="100"/>
+      <c r="R28" s="99"/>
       <c r="S28" s="7" t="s">
         <v>48</v>
       </c>
@@ -7666,7 +7665,7 @@
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="F29" s="1"/>
-      <c r="R29" s="100"/>
+      <c r="R29" s="99"/>
       <c r="S29" s="7" t="s">
         <v>49</v>
       </c>
@@ -7704,7 +7703,7 @@
         <f>K27+SUM(J15:J20)+SUM(AK5:AK12)</f>
         <v>5.3991399213407433E-2</v>
       </c>
-      <c r="R30" s="100"/>
+      <c r="R30" s="99"/>
       <c r="S30" s="7" t="s">
         <v>50</v>
       </c>
@@ -7748,7 +7747,7 @@
         <f>( 0.000001*14) / 0.151</f>
         <v>9.2715231788079476E-5</v>
       </c>
-      <c r="R31" s="100"/>
+      <c r="R31" s="99"/>
       <c r="S31" s="7" t="s">
         <v>51</v>
       </c>
@@ -7795,7 +7794,7 @@
         <f>E26*E31+F26*F31</f>
         <v>0</v>
       </c>
-      <c r="R32" s="100"/>
+      <c r="R32" s="99"/>
       <c r="S32" s="9" t="s">
         <v>52</v>
       </c>
@@ -7834,7 +7833,7 @@
       </c>
     </row>
     <row r="35" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="101" t="s">
+      <c r="A35" s="100" t="s">
         <v>152</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -7883,7 +7882,7 @@
       <c r="Q35" s="27"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A36" s="101"/>
+      <c r="A36" s="100"/>
       <c r="B36">
         <v>1</v>
       </c>
@@ -8008,7 +8007,7 @@
   </sheetPr>
   <dimension ref="A1:BD66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF4" workbookViewId="0">
+    <sheetView topLeftCell="AF4" workbookViewId="0">
       <selection activeCell="AK15" sqref="AK15"/>
     </sheetView>
   </sheetViews>
@@ -8032,8 +8031,8 @@
       <c r="E1" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="W1" s="93"/>
-      <c r="X1" s="94"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="93"/>
     </row>
     <row r="2" spans="1:56" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="52" t="s">
@@ -8047,11 +8046,11 @@
         <f xml:space="preserve"> 76.1/12*24*3600</f>
         <v>547920</v>
       </c>
-      <c r="W2" s="95"/>
-      <c r="X2" s="95"/>
+      <c r="W2" s="94"/>
+      <c r="X2" s="94"/>
     </row>
     <row r="4" spans="1:56" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="98" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -8118,7 +8117,7 @@
         <v>13</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="X4" s="5" t="s">
         <v>14</v>
@@ -8171,8 +8170,8 @@
       <c r="AN4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AO4" s="97" t="s">
-        <v>179</v>
+      <c r="AO4" s="96" t="s">
+        <v>177</v>
       </c>
       <c r="AP4" s="12" t="s">
         <v>77</v>
@@ -8190,13 +8189,13 @@
         <v>24</v>
       </c>
       <c r="AU4" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="AV4" s="86" t="s">
-        <v>162</v>
-      </c>
-      <c r="AW4" s="86" t="s">
-        <v>170</v>
+        <v>159</v>
+      </c>
+      <c r="AV4" s="85" t="s">
+        <v>160</v>
+      </c>
+      <c r="AW4" s="85" t="s">
+        <v>168</v>
       </c>
       <c r="AX4" s="6" t="s">
         <v>63</v>
@@ -8219,7 +8218,7 @@
       </c>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A5" s="99"/>
+      <c r="A5" s="98"/>
       <c r="B5">
         <v>1</v>
       </c>
@@ -8362,7 +8361,7 @@
         <f t="shared" ref="AP5:AP34" si="4">AK5+(AE5+AG5)*$E$53+AF5*$F$53+AH5*$J$53</f>
         <v>3.5556897359839751E-3</v>
       </c>
-      <c r="AQ5" s="89">
+      <c r="AQ5" s="88">
         <f t="shared" ref="AQ5:AQ34" si="5">(1-AK5/AP5)*100</f>
         <v>43.208264858268919</v>
       </c>
@@ -8414,7 +8413,7 @@
       </c>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A6" s="99"/>
+      <c r="A6" s="98"/>
       <c r="B6">
         <v>1</v>
       </c>
@@ -8557,7 +8556,7 @@
         <f t="shared" si="4"/>
         <v>1.2026079782581291E-3</v>
       </c>
-      <c r="AQ6" s="89">
+      <c r="AQ6" s="88">
         <f t="shared" si="5"/>
         <v>57.725997070438204</v>
       </c>
@@ -8609,7 +8608,7 @@
       </c>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A7" s="99"/>
+      <c r="A7" s="98"/>
       <c r="B7">
         <v>1</v>
       </c>
@@ -8751,7 +8750,7 @@
         <f t="shared" si="4"/>
         <v>3.4867252364606023E-5</v>
       </c>
-      <c r="AQ7" s="89">
+      <c r="AQ7" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -8801,7 +8800,7 @@
       </c>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A8" s="99"/>
+      <c r="A8" s="98"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -8943,7 +8942,7 @@
         <f t="shared" si="4"/>
         <v>9.4896679346414427E-6</v>
       </c>
-      <c r="AQ8" s="89">
+      <c r="AQ8" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -8993,7 +8992,7 @@
       </c>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A9" s="99"/>
+      <c r="A9" s="98"/>
       <c r="B9">
         <v>1</v>
       </c>
@@ -9135,7 +9134,7 @@
         <f t="shared" si="4"/>
         <v>3.281569422499217E-6</v>
       </c>
-      <c r="AQ9" s="89">
+      <c r="AQ9" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -9185,7 +9184,7 @@
       </c>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A10" s="99"/>
+      <c r="A10" s="98"/>
       <c r="B10">
         <v>1</v>
       </c>
@@ -9327,7 +9326,7 @@
         <f t="shared" si="4"/>
         <v>1.4545476567305404E-6</v>
       </c>
-      <c r="AQ10" s="89">
+      <c r="AQ10" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -9377,7 +9376,7 @@
       </c>
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A11" s="99"/>
+      <c r="A11" s="98"/>
       <c r="B11">
         <v>1</v>
       </c>
@@ -9519,7 +9518,7 @@
         <f t="shared" si="4"/>
         <v>5.5878867222163193E-7</v>
       </c>
-      <c r="AQ11" s="89">
+      <c r="AQ11" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -9569,7 +9568,7 @@
       </c>
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A12" s="99"/>
+      <c r="A12" s="98"/>
       <c r="B12">
         <v>1</v>
       </c>
@@ -9711,7 +9710,7 @@
         <f t="shared" si="4"/>
         <v>3.9214700262632978E-7</v>
       </c>
-      <c r="AQ12" s="89">
+      <c r="AQ12" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -9761,7 +9760,7 @@
       </c>
     </row>
     <row r="13" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A13" s="99"/>
+      <c r="A13" s="98"/>
       <c r="B13">
         <f>B6</f>
         <v>1</v>
@@ -9925,7 +9924,7 @@
         <f t="shared" si="4"/>
         <v>1.2026079782581291E-3</v>
       </c>
-      <c r="AQ13" s="89">
+      <c r="AQ13" s="88">
         <f t="shared" si="5"/>
         <v>57.725997070438204</v>
       </c>
@@ -9961,7 +9960,7 @@
       <c r="BD13" s="7"/>
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A14" s="99"/>
+      <c r="A14" s="98"/>
       <c r="B14">
         <f t="shared" ref="B14:B19" si="27">B7</f>
         <v>1</v>
@@ -10125,7 +10124,7 @@
         <f t="shared" si="4"/>
         <v>3.4867252364606023E-5</v>
       </c>
-      <c r="AQ14" s="89">
+      <c r="AQ14" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -10162,7 +10161,7 @@
       <c r="BD14" s="7"/>
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A15" s="99"/>
+      <c r="A15" s="98"/>
       <c r="B15">
         <f t="shared" si="27"/>
         <v>1</v>
@@ -10326,7 +10325,7 @@
         <f t="shared" si="4"/>
         <v>9.4896679346414427E-6</v>
       </c>
-      <c r="AQ15" s="89">
+      <c r="AQ15" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -10363,7 +10362,7 @@
       <c r="BD15" s="7"/>
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A16" s="99"/>
+      <c r="A16" s="98"/>
       <c r="B16">
         <f t="shared" si="27"/>
         <v>1</v>
@@ -10527,7 +10526,7 @@
         <f t="shared" si="4"/>
         <v>3.281569422499217E-6</v>
       </c>
-      <c r="AQ16" s="89">
+      <c r="AQ16" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -10564,7 +10563,7 @@
       <c r="BD16" s="7"/>
     </row>
     <row r="17" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A17" s="99"/>
+      <c r="A17" s="98"/>
       <c r="B17">
         <f t="shared" si="27"/>
         <v>1</v>
@@ -10728,7 +10727,7 @@
         <f t="shared" si="4"/>
         <v>1.4545476567305404E-6</v>
       </c>
-      <c r="AQ17" s="89">
+      <c r="AQ17" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -10765,7 +10764,7 @@
       <c r="BD17" s="7"/>
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A18" s="99"/>
+      <c r="A18" s="98"/>
       <c r="B18">
         <f t="shared" si="27"/>
         <v>1</v>
@@ -10929,7 +10928,7 @@
         <f t="shared" si="4"/>
         <v>5.5878867222163193E-7</v>
       </c>
-      <c r="AQ18" s="89">
+      <c r="AQ18" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -10966,7 +10965,7 @@
       <c r="BD18" s="7"/>
     </row>
     <row r="19" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A19" s="99"/>
+      <c r="A19" s="98"/>
       <c r="B19">
         <f t="shared" si="27"/>
         <v>1</v>
@@ -11130,7 +11129,7 @@
         <f t="shared" si="4"/>
         <v>3.9214700262632978E-7</v>
       </c>
-      <c r="AQ19" s="89">
+      <c r="AQ19" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -11167,7 +11166,7 @@
       <c r="BD19" s="7"/>
     </row>
     <row r="20" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A20" s="99"/>
+      <c r="A20" s="98"/>
       <c r="B20">
         <f>B7</f>
         <v>1</v>
@@ -11331,7 +11330,7 @@
         <f t="shared" si="4"/>
         <v>3.4867252364606023E-5</v>
       </c>
-      <c r="AQ20" s="89">
+      <c r="AQ20" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -11368,7 +11367,7 @@
       <c r="BD20" s="7"/>
     </row>
     <row r="21" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A21" s="99"/>
+      <c r="A21" s="98"/>
       <c r="B21">
         <f t="shared" ref="B21:B34" si="67">B8</f>
         <v>1</v>
@@ -11532,7 +11531,7 @@
         <f t="shared" si="4"/>
         <v>9.4896679346414427E-6</v>
       </c>
-      <c r="AQ21" s="89">
+      <c r="AQ21" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -11569,7 +11568,7 @@
       <c r="BD21" s="7"/>
     </row>
     <row r="22" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A22" s="99"/>
+      <c r="A22" s="98"/>
       <c r="B22">
         <f t="shared" si="67"/>
         <v>1</v>
@@ -11733,7 +11732,7 @@
         <f t="shared" si="4"/>
         <v>3.281569422499217E-6</v>
       </c>
-      <c r="AQ22" s="89">
+      <c r="AQ22" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -11770,7 +11769,7 @@
       <c r="BD22" s="7"/>
     </row>
     <row r="23" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A23" s="99"/>
+      <c r="A23" s="98"/>
       <c r="B23">
         <f t="shared" si="67"/>
         <v>1</v>
@@ -11934,7 +11933,7 @@
         <f t="shared" si="4"/>
         <v>1.4545476567305404E-6</v>
       </c>
-      <c r="AQ23" s="89">
+      <c r="AQ23" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -11971,7 +11970,7 @@
       <c r="BD23" s="7"/>
     </row>
     <row r="24" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A24" s="99"/>
+      <c r="A24" s="98"/>
       <c r="B24">
         <f t="shared" si="67"/>
         <v>1</v>
@@ -12135,7 +12134,7 @@
         <f t="shared" si="4"/>
         <v>5.5878867222163193E-7</v>
       </c>
-      <c r="AQ24" s="89">
+      <c r="AQ24" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -12172,7 +12171,7 @@
       <c r="BD24" s="7"/>
     </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A25" s="99"/>
+      <c r="A25" s="98"/>
       <c r="B25">
         <f t="shared" si="67"/>
         <v>1</v>
@@ -12336,7 +12335,7 @@
         <f t="shared" si="4"/>
         <v>3.9214700262632978E-7</v>
       </c>
-      <c r="AQ25" s="89">
+      <c r="AQ25" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -12373,7 +12372,7 @@
       <c r="BD25" s="7"/>
     </row>
     <row r="26" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A26" s="99"/>
+      <c r="A26" s="98"/>
       <c r="B26">
         <f t="shared" si="67"/>
         <v>1</v>
@@ -12537,7 +12536,7 @@
         <f t="shared" si="4"/>
         <v>9.4896679346414427E-6</v>
       </c>
-      <c r="AQ26" s="89">
+      <c r="AQ26" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -12574,7 +12573,7 @@
       <c r="BD26" s="7"/>
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A27" s="99"/>
+      <c r="A27" s="98"/>
       <c r="B27">
         <f t="shared" si="67"/>
         <v>1</v>
@@ -12738,7 +12737,7 @@
         <f t="shared" si="4"/>
         <v>3.281569422499217E-6</v>
       </c>
-      <c r="AQ27" s="89">
+      <c r="AQ27" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -12775,7 +12774,7 @@
       <c r="BD27" s="7"/>
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A28" s="99"/>
+      <c r="A28" s="98"/>
       <c r="B28">
         <f t="shared" si="67"/>
         <v>1</v>
@@ -12939,7 +12938,7 @@
         <f t="shared" si="4"/>
         <v>1.4545476567305404E-6</v>
       </c>
-      <c r="AQ28" s="89">
+      <c r="AQ28" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -12976,7 +12975,7 @@
       <c r="BD28" s="7"/>
     </row>
     <row r="29" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A29" s="99"/>
+      <c r="A29" s="98"/>
       <c r="B29">
         <f t="shared" si="67"/>
         <v>1</v>
@@ -13140,7 +13139,7 @@
         <f t="shared" si="4"/>
         <v>5.5878867222163193E-7</v>
       </c>
-      <c r="AQ29" s="89">
+      <c r="AQ29" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -13177,7 +13176,7 @@
       <c r="BD29" s="7"/>
     </row>
     <row r="30" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A30" s="99"/>
+      <c r="A30" s="98"/>
       <c r="B30">
         <f t="shared" si="67"/>
         <v>1</v>
@@ -13341,7 +13340,7 @@
         <f t="shared" si="4"/>
         <v>3.9214700262632978E-7</v>
       </c>
-      <c r="AQ30" s="89">
+      <c r="AQ30" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -13378,7 +13377,7 @@
       <c r="BD30" s="7"/>
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A31" s="99"/>
+      <c r="A31" s="98"/>
       <c r="B31">
         <f t="shared" si="67"/>
         <v>1</v>
@@ -13542,7 +13541,7 @@
         <f t="shared" si="4"/>
         <v>3.281569422499217E-6</v>
       </c>
-      <c r="AQ31" s="89">
+      <c r="AQ31" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -13579,7 +13578,7 @@
       <c r="BD31" s="7"/>
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A32" s="99"/>
+      <c r="A32" s="98"/>
       <c r="B32">
         <f t="shared" si="67"/>
         <v>1</v>
@@ -13743,7 +13742,7 @@
         <f t="shared" si="4"/>
         <v>1.4545476567305404E-6</v>
       </c>
-      <c r="AQ32" s="89">
+      <c r="AQ32" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -13780,7 +13779,7 @@
       <c r="BD32" s="7"/>
     </row>
     <row r="33" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A33" s="99"/>
+      <c r="A33" s="98"/>
       <c r="B33">
         <f t="shared" si="67"/>
         <v>1</v>
@@ -13944,7 +13943,7 @@
         <f t="shared" si="4"/>
         <v>5.5878867222163193E-7</v>
       </c>
-      <c r="AQ33" s="89">
+      <c r="AQ33" s="88">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -13981,7 +13980,7 @@
       <c r="BD33" s="7"/>
     </row>
     <row r="34" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A34" s="99"/>
+      <c r="A34" s="98"/>
       <c r="B34">
         <f t="shared" si="67"/>
         <v>1</v>
@@ -14145,7 +14144,7 @@
         <f t="shared" si="4"/>
         <v>3.9214700262632978E-7</v>
       </c>
-      <c r="AQ34" s="90">
+      <c r="AQ34" s="89">
         <f t="shared" si="5"/>
         <v>67.910893172283792</v>
       </c>
@@ -14194,7 +14193,7 @@
       <c r="AF35" s="1"/>
     </row>
     <row r="36" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="99" t="s">
+      <c r="A36" s="98" t="s">
         <v>71</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -14296,7 +14295,7 @@
       <c r="AV36" s="40"/>
     </row>
     <row r="37" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A37" s="99"/>
+      <c r="A37" s="98"/>
       <c r="B37">
         <v>1</v>
       </c>
@@ -14417,12 +14416,12 @@
         <f>AR37+AQ37</f>
         <v>11764.705882352941</v>
       </c>
-      <c r="AT37" s="84"/>
-      <c r="AU37" s="84"/>
-      <c r="AV37" s="84"/>
+      <c r="AT37" s="83"/>
+      <c r="AU37" s="83"/>
+      <c r="AV37" s="83"/>
     </row>
     <row r="38" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A38" s="99"/>
+      <c r="A38" s="98"/>
       <c r="B38">
         <v>1</v>
       </c>
@@ -14545,12 +14544,12 @@
         <f>AR38+AQ38</f>
         <v>20</v>
       </c>
-      <c r="AT38" s="85"/>
-      <c r="AU38" s="85"/>
-      <c r="AV38" s="85"/>
+      <c r="AT38" s="84"/>
+      <c r="AU38" s="84"/>
+      <c r="AV38" s="84"/>
     </row>
     <row r="39" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A39" s="99"/>
+      <c r="A39" s="98"/>
       <c r="B39">
         <v>1</v>
       </c>
@@ -14656,7 +14655,7 @@
       <c r="AG39" s="1"/>
     </row>
     <row r="40" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A40" s="99"/>
+      <c r="A40" s="98"/>
       <c r="B40">
         <v>1</v>
       </c>
@@ -14762,7 +14761,7 @@
       <c r="AG40" s="1"/>
     </row>
     <row r="41" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A41" s="99"/>
+      <c r="A41" s="98"/>
       <c r="B41">
         <v>1</v>
       </c>
@@ -14873,7 +14872,7 @@
       </c>
     </row>
     <row r="42" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A42" s="99"/>
+      <c r="A42" s="98"/>
       <c r="B42">
         <v>1</v>
       </c>
@@ -14986,14 +14985,14 @@
       <c r="X43" s="15"/>
       <c r="Z43" s="1"/>
       <c r="AN43" s="78"/>
-      <c r="AO43" s="96"/>
+      <c r="AO43" s="95"/>
       <c r="AP43" s="78"/>
       <c r="AQ43" s="78"/>
       <c r="AR43" s="78"/>
       <c r="AS43" s="78"/>
-      <c r="AT43" s="83"/>
-      <c r="AU43" s="83"/>
-      <c r="AV43" s="92"/>
+      <c r="AT43" s="82"/>
+      <c r="AU43" s="82"/>
+      <c r="AV43" s="91"/>
       <c r="AW43" s="7" t="s">
         <v>49</v>
       </c>
@@ -15014,18 +15013,18 @@
       <c r="AA44" s="42">
         <v>5</v>
       </c>
-      <c r="AC44" s="87" t="s">
-        <v>163</v>
+      <c r="AC44" s="86" t="s">
+        <v>161</v>
       </c>
       <c r="AN44" s="78"/>
-      <c r="AO44" s="96"/>
+      <c r="AO44" s="95"/>
       <c r="AP44" s="78"/>
       <c r="AQ44" s="78"/>
       <c r="AR44" s="78"/>
       <c r="AS44" s="78"/>
-      <c r="AT44" s="83"/>
-      <c r="AU44" s="83"/>
-      <c r="AV44" s="92"/>
+      <c r="AT44" s="82"/>
+      <c r="AU44" s="82"/>
+      <c r="AV44" s="91"/>
       <c r="AW44" s="7" t="s">
         <v>50</v>
       </c>
@@ -15046,18 +15045,18 @@
       <c r="AA45" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="AC45" s="88">
+      <c r="AC45" s="87">
         <v>200</v>
       </c>
       <c r="AN45" s="78"/>
-      <c r="AO45" s="96"/>
+      <c r="AO45" s="95"/>
       <c r="AP45" s="78"/>
       <c r="AQ45" s="78"/>
       <c r="AR45" s="78"/>
       <c r="AS45" s="78"/>
-      <c r="AT45" s="83"/>
-      <c r="AU45" s="83"/>
-      <c r="AV45" s="92"/>
+      <c r="AT45" s="82"/>
+      <c r="AU45" s="82"/>
+      <c r="AV45" s="91"/>
       <c r="AW45" s="7" t="s">
         <v>60</v>
       </c>
@@ -15087,7 +15086,7 @@
       </c>
     </row>
     <row r="47" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A47" s="99" t="s">
+      <c r="A47" s="98" t="s">
         <v>72</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -15144,7 +15143,7 @@
       </c>
     </row>
     <row r="48" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A48" s="99"/>
+      <c r="A48" s="98"/>
       <c r="B48">
         <v>1</v>
       </c>
@@ -15194,7 +15193,7 @@
       <c r="AW48" s="7"/>
     </row>
     <row r="49" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A49" s="99"/>
+      <c r="A49" s="98"/>
       <c r="B49">
         <v>1</v>
       </c>
@@ -15249,7 +15248,7 @@
       <c r="Q49" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="R49" s="100" t="s">
+      <c r="R49" s="99" t="s">
         <v>46</v>
       </c>
       <c r="S49" s="7" t="s">
@@ -15308,7 +15307,7 @@
         <f>INPUTS!Q28</f>
         <v>1.2</v>
       </c>
-      <c r="R50" s="100"/>
+      <c r="R50" s="99"/>
       <c r="S50" s="7" t="s">
         <v>48</v>
       </c>
@@ -15331,7 +15330,7 @@
     </row>
     <row r="51" spans="1:49" x14ac:dyDescent="0.25">
       <c r="F51" s="1"/>
-      <c r="R51" s="100"/>
+      <c r="R51" s="99"/>
       <c r="S51" s="7" t="s">
         <v>49</v>
       </c>
@@ -15370,7 +15369,7 @@
         <f>K49+SUM(J37:J42)+SUM(AK5:AK34)</f>
         <v>5.4681379650622607E-2</v>
       </c>
-      <c r="R52" s="100"/>
+      <c r="R52" s="99"/>
       <c r="S52" s="7" t="s">
         <v>50</v>
       </c>
@@ -15415,7 +15414,7 @@
         <f>( 0.000001*14) / 0.151</f>
         <v>9.2715231788079476E-5</v>
       </c>
-      <c r="R53" s="100"/>
+      <c r="R53" s="99"/>
       <c r="S53" s="7" t="s">
         <v>51</v>
       </c>
@@ -15463,7 +15462,7 @@
         <f>E48*E53+F48*F53</f>
         <v>0</v>
       </c>
-      <c r="R54" s="100"/>
+      <c r="R54" s="99"/>
       <c r="S54" s="9" t="s">
         <v>52</v>
       </c>
@@ -15502,7 +15501,7 @@
       </c>
     </row>
     <row r="57" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="102" t="s">
+      <c r="A57" s="101" t="s">
         <v>152</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -15551,7 +15550,7 @@
       <c r="Q57" s="27"/>
     </row>
     <row r="58" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A58" s="102"/>
+      <c r="A58" s="101"/>
       <c r="B58">
         <v>1</v>
       </c>
@@ -15593,7 +15592,7 @@
       <c r="Q58" s="1"/>
     </row>
     <row r="59" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A59" s="102"/>
+      <c r="A59" s="101"/>
       <c r="B59">
         <f>B58</f>
         <v>1</v>
@@ -15649,7 +15648,7 @@
       </c>
     </row>
     <row r="60" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A60" s="102"/>
+      <c r="A60" s="101"/>
       <c r="B60">
         <f>B59</f>
         <v>1</v>
@@ -15705,7 +15704,7 @@
       </c>
     </row>
     <row r="61" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A61" s="102"/>
+      <c r="A61" s="101"/>
       <c r="B61">
         <f>B60</f>
         <v>1</v>
@@ -15761,7 +15760,7 @@
       </c>
     </row>
     <row r="62" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A62" s="102"/>
+      <c r="A62" s="101"/>
       <c r="B62">
         <f>B61</f>
         <v>1</v>
@@ -15864,8 +15863,8 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15875,23 +15874,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="90" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="91" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" s="91" t="s">
+      <c r="C1" s="90" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="90" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="90" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="91" t="s">
-        <v>159</v>
-      </c>
-      <c r="F1" s="91" t="s">
-        <v>160</v>
-      </c>
       <c r="I1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -15905,23 +15904,23 @@
         <f>B2*10^3/10000</f>
         <v>6</v>
       </c>
-      <c r="D2" s="81">
+      <c r="D2" s="1">
         <f>C2*10^6/14</f>
         <v>428571.42857142858</v>
       </c>
-      <c r="E2" s="82">
+      <c r="E2" s="81">
         <v>36146</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -15930,11 +15929,11 @@
         <f t="shared" ref="C3:C4" si="0">B3*10^3/10000</f>
         <v>5</v>
       </c>
-      <c r="D3" s="81">
+      <c r="D3" s="1">
         <f t="shared" ref="D3:D4" si="1">C3*10^6/14</f>
         <v>357142.85714285716</v>
       </c>
-      <c r="E3" s="82">
+      <c r="E3" s="81">
         <v>36230</v>
       </c>
       <c r="F3">
@@ -15942,12 +15941,12 @@
         <v>2016</v>
       </c>
       <c r="I3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4">
         <v>140</v>
@@ -15956,11 +15955,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <f t="shared" si="1"/>
         <v>1000000</v>
       </c>
-      <c r="E4" s="82">
+      <c r="E4" s="81">
         <v>36251</v>
       </c>
       <c r="F4">
@@ -15968,11 +15967,11 @@
         <v>2520</v>
       </c>
       <c r="I4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E5" s="82"/>
+      <c r="E5" s="81"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16407,7 +16406,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D18">
         <v>58</v>
@@ -16417,7 +16416,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D19">
         <v>106</v>
@@ -16446,7 +16445,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D21">
         <v>75</v>
@@ -16500,10 +16499,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D1">
         <f>1/0.15</f>
@@ -16512,7 +16511,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>